<commit_message>
add phase 6 + small redesign
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebiru\code\Informatik-2.Jahr\IPT6.1\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B44F1C-44FE-404D-AE98-CE98A79BDC64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B60A9-7783-4C5A-9D90-F6CE497B839E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4785" yWindow="-21600" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Productivity-Game</t>
   </si>
   <si>
-    <t>Phase 1.1: Projektdefinition</t>
-  </si>
-  <si>
     <t>Ziel der Anwendung schriftlich festhalten</t>
   </si>
   <si>
@@ -106,9 +103,6 @@
     <t>Tasksverwaltung</t>
   </si>
   <si>
-    <t>Phase 1.2: Feature-Liste &amp; Use-Cases</t>
-  </si>
-  <si>
     <t>Features auflisten (CRUD)</t>
   </si>
   <si>
@@ -124,9 +118,6 @@
     <t>Wichtige Use-Cases beschreiben </t>
   </si>
   <si>
-    <t>Phase 1.3: Datenanalyse &amp; Modellierung</t>
-  </si>
-  <si>
     <t>Entitäten definieren</t>
   </si>
   <si>
@@ -136,24 +127,15 @@
     <t>Relationales Datenbankmodell erstellen</t>
   </si>
   <si>
-    <t>Phase 1.4: OOP-Design</t>
-  </si>
-  <si>
     <t>Klassen definieren passend zur DB</t>
   </si>
   <si>
     <t>UML-Klassendiagramm erstellen</t>
   </si>
   <si>
-    <t>Phase: 1.5: Programmablauf planen</t>
-  </si>
-  <si>
     <t>PAP erstellen (PapDesigner)</t>
   </si>
   <si>
-    <t>Phase 2.1: Seitenstruktur</t>
-  </si>
-  <si>
     <t>Seiten festlegen</t>
   </si>
   <si>
@@ -166,9 +148,6 @@
     <t>Benutzerabläufe festlegen</t>
   </si>
   <si>
-    <t>Phase 2.2: Wireframes</t>
-  </si>
-  <si>
     <t>Wireframe-Tool auswählen</t>
   </si>
   <si>
@@ -214,15 +193,6 @@
     <t>Diagramme ablegen</t>
   </si>
   <si>
-    <t>Phase 2.4: Datenmodell (DB)</t>
-  </si>
-  <si>
-    <t>Phase 2.3: Mockup-Erstellung</t>
-  </si>
-  <si>
-    <t>Phase 3.1: Grundsetup</t>
-  </si>
-  <si>
     <t>SQLite Scripte erstellen (Create, Insert, Programmability)</t>
   </si>
   <si>
@@ -241,9 +211,6 @@
     <t>Fehlerbehandlung für Datenbankzugriffe integrieren</t>
   </si>
   <si>
-    <t>Phase 3.2: Authentifizierung</t>
-  </si>
-  <si>
     <t>Benutzer anlegen</t>
   </si>
   <si>
@@ -256,9 +223,6 @@
     <t>Validierung von Benutzereingaben</t>
   </si>
   <si>
-    <t>Phase 3.3: Task-Logik</t>
-  </si>
-  <si>
     <t>CRUD-Funktionalität für Tasks implementieren</t>
   </si>
   <si>
@@ -268,9 +232,6 @@
     <t>Erledigte Tasks in der Datenbank protokollieren(TaskLog)</t>
   </si>
   <si>
-    <t>Phase 4.1: XP-System</t>
-  </si>
-  <si>
     <t>XP-Regeln festlegen (Formel/Faktoren)</t>
   </si>
   <si>
@@ -283,9 +244,6 @@
     <t>Gesamt-XP pro User berechnen/abrufend</t>
   </si>
   <si>
-    <t>Phase 4.2: Level System</t>
-  </si>
-  <si>
     <t>Level Grenzen definieren</t>
   </si>
   <si>
@@ -301,9 +259,6 @@
     <t>Belohnungen vorbereiten (Badges usw.)</t>
   </si>
   <si>
-    <t>Phase 4.3: Streaks</t>
-  </si>
-  <si>
     <t>Regeln definieren</t>
   </si>
   <si>
@@ -316,9 +271,6 @@
     <t>Streak Status speichern</t>
   </si>
   <si>
-    <t>Phase 5.1: Grundlayout</t>
-  </si>
-  <si>
     <t>Vue Projekt erstellen</t>
   </si>
   <si>
@@ -365,6 +317,93 @@
   </si>
   <si>
     <t>Nach erledigter Task Feedback zurückgeben</t>
+  </si>
+  <si>
+    <t>Phase 1: Planung &amp; Vorbereitung                        1.1: Projektdefinition</t>
+  </si>
+  <si>
+    <t>1.2: Feature-Liste &amp; Use-Cases</t>
+  </si>
+  <si>
+    <t>1.3: Datenanalyse &amp; Modellierung</t>
+  </si>
+  <si>
+    <t>1.4: OOP-Design</t>
+  </si>
+  <si>
+    <t>1.5: Programmablauf planen</t>
+  </si>
+  <si>
+    <t>Phase 2: UX/UI &amp; Struktur                                        2.1: Seitenstruktur</t>
+  </si>
+  <si>
+    <t>2.2: Wireframes</t>
+  </si>
+  <si>
+    <t>2.3: Mockup-Erstellung</t>
+  </si>
+  <si>
+    <t>2.4: Datenmodell (DB)</t>
+  </si>
+  <si>
+    <t>3.2: Authentifizierung</t>
+  </si>
+  <si>
+    <t>3.3: Task-Logik</t>
+  </si>
+  <si>
+    <t>Phase 4: Gamification-Logik                                   4.1: XP-System</t>
+  </si>
+  <si>
+    <t>Phase 3: Backend/DB - Basis                                   3.1: Grundsetup</t>
+  </si>
+  <si>
+    <t>4.2: Level System</t>
+  </si>
+  <si>
+    <t>4.3: Streaks</t>
+  </si>
+  <si>
+    <t>Phase 5: Frontend – Kernfunktionen                  5.1: Grundlayout</t>
+  </si>
+  <si>
+    <t>Phase 6: Dashboard &amp; Statistiken                          6.1 Dashboard</t>
+  </si>
+  <si>
+    <t>Festlegen welche Informationen angezeigt werden sollen</t>
+  </si>
+  <si>
+    <t>Zentrales Dashboard umsetzen</t>
+  </si>
+  <si>
+    <t>Kurze Zusammenfassung der letzten Aktivitäten</t>
+  </si>
+  <si>
+    <t>Schneller Zugriff auf wichtige Funktionen/Aktionen</t>
+  </si>
+  <si>
+    <t>6.2 Diagramme</t>
+  </si>
+  <si>
+    <t>Produktivitätsdiagramme anzeigen</t>
+  </si>
+  <si>
+    <t>Zeitraum-Filter implementieren</t>
+  </si>
+  <si>
+    <t>Daten aus der Datenbank leiten</t>
+  </si>
+  <si>
+    <t>Diagramme übersichtlich und verständlich darstellen</t>
+  </si>
+  <si>
+    <t>6.3 Heatmaps (optional)</t>
+  </si>
+  <si>
+    <t>Produktive Zeiten visualisieren</t>
+  </si>
+  <si>
+    <t>Erledigte Tasks zeitlich auswerten</t>
   </si>
 </sst>
 </file>
@@ -735,7 +774,27 @@
     <cellStyle name="Task Indicator" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="5" tint="-0.499984740745262"/>
@@ -837,10 +896,10 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Idea Planner" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Idea Planner" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="10"/>
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="firstColumn" dxfId="8"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="firstColumn" dxfId="11"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="10"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -910,8 +969,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G101" totalsRowShown="0">
-  <autoFilter ref="B6:G101" xr:uid="{00000000-0009-0000-0100-000001000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tasks" displayName="Tasks" ref="B6:G115" totalsRowShown="0">
+  <autoFilter ref="B6:G115" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -929,7 +988,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status Icon" dataCellStyle="Status Icon Text">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1209,10 +1268,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G101"/>
+  <dimension ref="B1:G115"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1307,7 +1366,7 @@
         <v/>
       </c>
       <c r="C7" s="14" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
@@ -1326,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="7">
         <f ca="1">TODAY()</f>
@@ -1347,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="7">
         <f ca="1">TODAY()</f>
@@ -1368,7 +1427,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="7">
         <f ca="1">TODAY()</f>
@@ -1389,7 +1448,7 @@
         <v/>
       </c>
       <c r="C11" s="18" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="20"/>
@@ -1405,7 +1464,7 @@
         <v>-1</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D12" s="12">
         <v>46078</v>
@@ -1425,7 +1484,7 @@
         <v>-1</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D13" s="12">
         <v>46078</v>
@@ -1445,7 +1504,7 @@
         <v>-1</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D14" s="12">
         <v>46078</v>
@@ -1465,7 +1524,7 @@
         <v>-1</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" s="12">
         <v>46078</v>
@@ -1485,7 +1544,7 @@
         <v>-1</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="12">
         <v>46078</v>
@@ -1505,7 +1564,7 @@
         <v/>
       </c>
       <c r="C17" s="22" t="s">
-        <v>26</v>
+        <v>93</v>
       </c>
       <c r="D17" s="23"/>
       <c r="E17" s="24"/>
@@ -1521,7 +1580,7 @@
         <v>-1</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D18" s="12">
         <v>46078</v>
@@ -1541,7 +1600,7 @@
         <v>-1</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D19" s="12">
         <v>46078</v>
@@ -1561,7 +1620,7 @@
         <v>-1</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D20" s="12">
         <v>46078</v>
@@ -1581,7 +1640,7 @@
         <v/>
       </c>
       <c r="C21" s="22" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="D21" s="23"/>
       <c r="E21" s="24"/>
@@ -1597,7 +1656,7 @@
         <v>-1</v>
       </c>
       <c r="C22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D22" s="12">
         <v>46078</v>
@@ -1617,7 +1676,7 @@
         <v>-1</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D23" s="12">
         <v>46078</v>
@@ -1637,7 +1696,7 @@
         <v/>
       </c>
       <c r="C24" s="22" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="D24" s="23"/>
       <c r="E24" s="24"/>
@@ -1653,7 +1712,7 @@
         <v>-1</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D25" s="12">
         <v>46078</v>
@@ -1673,7 +1732,7 @@
         <v/>
       </c>
       <c r="C26" s="14" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="D26" s="31"/>
       <c r="E26" s="32"/>
@@ -1689,7 +1748,7 @@
         <v/>
       </c>
       <c r="C27" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="13"/>
@@ -1705,7 +1764,7 @@
         <v/>
       </c>
       <c r="C28" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="13"/>
@@ -1721,7 +1780,7 @@
         <v/>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
@@ -1737,7 +1796,7 @@
         <v/>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="13"/>
@@ -1753,7 +1812,7 @@
         <v/>
       </c>
       <c r="C31" s="14" t="s">
-        <v>40</v>
+        <v>97</v>
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="32"/>
@@ -1769,7 +1828,7 @@
         <v/>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
@@ -1785,7 +1844,7 @@
         <v/>
       </c>
       <c r="C33" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="13"/>
@@ -1801,7 +1860,7 @@
         <v/>
       </c>
       <c r="C34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="13"/>
@@ -1817,7 +1876,7 @@
         <v/>
       </c>
       <c r="C35" s="14" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="D35" s="31"/>
       <c r="E35" s="32"/>
@@ -1833,7 +1892,7 @@
         <v/>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="13"/>
@@ -1849,7 +1908,7 @@
         <v/>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="13"/>
@@ -1865,7 +1924,7 @@
         <v/>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
@@ -1881,7 +1940,7 @@
         <v/>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="13"/>
@@ -1897,7 +1956,7 @@
         <v/>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
@@ -1913,7 +1972,7 @@
         <v/>
       </c>
       <c r="C41" s="14" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="D41" s="31"/>
       <c r="E41" s="32"/>
@@ -1929,7 +1988,7 @@
         <v/>
       </c>
       <c r="C42" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
@@ -1945,7 +2004,7 @@
         <v/>
       </c>
       <c r="C43" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="13"/>
@@ -1961,7 +2020,7 @@
         <v/>
       </c>
       <c r="C44" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="13"/>
@@ -1980,7 +2039,7 @@
         <v/>
       </c>
       <c r="C45" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="13"/>
@@ -1996,7 +2055,7 @@
         <v/>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D46" s="12"/>
       <c r="E46" s="13"/>
@@ -2012,7 +2071,7 @@
         <v/>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="13"/>
@@ -2028,7 +2087,7 @@
         <v/>
       </c>
       <c r="C48" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="13"/>
@@ -2044,7 +2103,7 @@
         <v/>
       </c>
       <c r="C49" s="22" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="D49" s="23"/>
       <c r="E49" s="24"/>
@@ -2060,7 +2119,7 @@
         <v/>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
@@ -2076,7 +2135,7 @@
         <v/>
       </c>
       <c r="C51" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="13"/>
@@ -2092,7 +2151,7 @@
         <v/>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="13"/>
@@ -2108,7 +2167,7 @@
         <v/>
       </c>
       <c r="C53" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="13"/>
@@ -2124,7 +2183,7 @@
         <v/>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
@@ -2140,7 +2199,7 @@
         <v/>
       </c>
       <c r="C55" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="13"/>
@@ -2156,7 +2215,7 @@
         <v/>
       </c>
       <c r="C56" s="22" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="D56" s="23"/>
       <c r="E56" s="24"/>
@@ -2172,7 +2231,7 @@
         <v/>
       </c>
       <c r="C57" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="13"/>
@@ -2188,7 +2247,7 @@
         <v/>
       </c>
       <c r="C58" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
@@ -2204,7 +2263,7 @@
         <v/>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="13"/>
@@ -2220,7 +2279,7 @@
         <v/>
       </c>
       <c r="C60" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13"/>
@@ -2236,7 +2295,7 @@
         <v/>
       </c>
       <c r="C61" s="22" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
       <c r="D61" s="23"/>
       <c r="E61" s="24"/>
@@ -2252,7 +2311,7 @@
         <v/>
       </c>
       <c r="C62" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
@@ -2268,7 +2327,7 @@
         <v/>
       </c>
       <c r="C63" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="13"/>
@@ -2284,7 +2343,7 @@
         <v/>
       </c>
       <c r="C64" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="13"/>
@@ -2300,7 +2359,7 @@
         <v/>
       </c>
       <c r="C65" s="22" t="s">
-        <v>74</v>
+        <v>102</v>
       </c>
       <c r="D65" s="23"/>
       <c r="E65" s="24"/>
@@ -2316,7 +2375,7 @@
         <v/>
       </c>
       <c r="C66" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13"/>
@@ -2332,7 +2391,7 @@
         <v/>
       </c>
       <c r="C67" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="13"/>
@@ -2348,7 +2407,7 @@
         <v/>
       </c>
       <c r="C68" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="13"/>
@@ -2364,7 +2423,7 @@
         <v/>
       </c>
       <c r="C69" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="13"/>
@@ -2380,7 +2439,7 @@
         <v/>
       </c>
       <c r="C70" s="22" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="D70" s="23"/>
       <c r="E70" s="24"/>
@@ -2396,7 +2455,7 @@
         <v/>
       </c>
       <c r="C71" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="13"/>
@@ -2412,7 +2471,7 @@
         <v/>
       </c>
       <c r="C72" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="13"/>
@@ -2428,7 +2487,7 @@
         <v/>
       </c>
       <c r="C73" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="13"/>
@@ -2444,7 +2503,7 @@
         <v/>
       </c>
       <c r="C74" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="13"/>
@@ -2460,7 +2519,7 @@
         <v/>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="13"/>
@@ -2476,7 +2535,7 @@
         <v/>
       </c>
       <c r="C76" s="22" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="D76" s="23"/>
       <c r="E76" s="24"/>
@@ -2492,7 +2551,7 @@
         <v/>
       </c>
       <c r="C77" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="13"/>
@@ -2508,7 +2567,7 @@
         <v/>
       </c>
       <c r="C78" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="13"/>
@@ -2524,7 +2583,7 @@
         <v/>
       </c>
       <c r="C79" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="13"/>
@@ -2540,7 +2599,7 @@
         <v/>
       </c>
       <c r="C80" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="13"/>
@@ -2556,7 +2615,7 @@
         <v/>
       </c>
       <c r="C81" s="22" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="24"/>
@@ -2572,7 +2631,7 @@
         <v/>
       </c>
       <c r="C82" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="13"/>
@@ -2588,7 +2647,7 @@
         <v/>
       </c>
       <c r="C83" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13"/>
@@ -2604,7 +2663,7 @@
         <v/>
       </c>
       <c r="C84" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="13"/>
@@ -2620,7 +2679,7 @@
         <v/>
       </c>
       <c r="C85" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D85" s="12"/>
       <c r="E85" s="13"/>
@@ -2636,7 +2695,7 @@
         <v/>
       </c>
       <c r="C86" s="22" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D86" s="23"/>
       <c r="E86" s="24"/>
@@ -2652,7 +2711,7 @@
         <v/>
       </c>
       <c r="C87" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="13"/>
@@ -2668,7 +2727,7 @@
         <v/>
       </c>
       <c r="C88" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="D88" s="12"/>
       <c r="E88" s="13"/>
@@ -2684,7 +2743,7 @@
         <v/>
       </c>
       <c r="C89" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="13"/>
@@ -2700,7 +2759,7 @@
         <v/>
       </c>
       <c r="C90" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="D90" s="12"/>
       <c r="E90" s="13"/>
@@ -2716,7 +2775,7 @@
         <v/>
       </c>
       <c r="C91" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="13"/>
@@ -2732,7 +2791,7 @@
         <v/>
       </c>
       <c r="C92" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="13"/>
@@ -2748,7 +2807,7 @@
         <v/>
       </c>
       <c r="C93" s="22" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="D93" s="23"/>
       <c r="E93" s="24"/>
@@ -2764,7 +2823,7 @@
         <v/>
       </c>
       <c r="C94" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="13"/>
@@ -2780,7 +2839,7 @@
         <v/>
       </c>
       <c r="C95" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="13"/>
@@ -2796,7 +2855,7 @@
         <v/>
       </c>
       <c r="C96" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="13"/>
@@ -2812,7 +2871,7 @@
         <v/>
       </c>
       <c r="C97" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="13"/>
@@ -2827,18 +2886,24 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="D98" s="12"/>
-      <c r="E98" s="13"/>
-      <c r="F98" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G98" s="27"/>
+      <c r="C98" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="D98" s="23"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G98" s="29"/>
     </row>
     <row r="99" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B99" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
+      </c>
+      <c r="C99" t="s">
+        <v>108</v>
       </c>
       <c r="D99" s="12"/>
       <c r="E99" s="13"/>
@@ -2853,6 +2918,9 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
+      <c r="C100" t="s">
+        <v>109</v>
+      </c>
       <c r="D100" s="12"/>
       <c r="E100" s="13"/>
       <c r="F100" s="11" t="str">
@@ -2866,6 +2934,9 @@
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
+      <c r="C101" t="s">
+        <v>110</v>
+      </c>
       <c r="D101" s="12"/>
       <c r="E101" s="13"/>
       <c r="F101" s="11" t="str">
@@ -2873,6 +2944,215 @@
         <v/>
       </c>
       <c r="G101" s="27"/>
+    </row>
+    <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B102" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C102" t="s">
+        <v>111</v>
+      </c>
+      <c r="D102" s="12"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G102" s="27"/>
+    </row>
+    <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B103" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C103" s="22" t="s">
+        <v>112</v>
+      </c>
+      <c r="D103" s="23"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G103" s="29"/>
+    </row>
+    <row r="104" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B104" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C104" t="s">
+        <v>113</v>
+      </c>
+      <c r="D104" s="12"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G104" s="27"/>
+    </row>
+    <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B105" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C105" t="s">
+        <v>114</v>
+      </c>
+      <c r="D105" s="12"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G105" s="27"/>
+    </row>
+    <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B106" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C106" t="s">
+        <v>115</v>
+      </c>
+      <c r="D106" s="12"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G106" s="27"/>
+    </row>
+    <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B107" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C107" t="s">
+        <v>116</v>
+      </c>
+      <c r="D107" s="12"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G107" s="27"/>
+    </row>
+    <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B108" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D108" s="23"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G108" s="29"/>
+    </row>
+    <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B109" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C109" t="s">
+        <v>118</v>
+      </c>
+      <c r="D109" s="12"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G109" s="27"/>
+    </row>
+    <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B110" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C110" t="s">
+        <v>119</v>
+      </c>
+      <c r="D110" s="12"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G110" s="27"/>
+    </row>
+    <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D111" s="12"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G111" s="27"/>
+    </row>
+    <row r="112" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B112" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D112" s="12"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G112" s="27"/>
+    </row>
+    <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B113" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D113" s="12"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G113" s="27"/>
+    </row>
+    <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B114" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D114" s="12"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G114" s="27"/>
+    </row>
+    <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B115" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="D115" s="12"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="11" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G115" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2883,7 +3163,7 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <conditionalFormatting sqref="B7:B101">
+  <conditionalFormatting sqref="B7:B115">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="-1"/>
@@ -2895,14 +3175,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F101">
-    <cfRule type="expression" dxfId="5" priority="5">
+  <conditionalFormatting sqref="F7:F115">
+    <cfRule type="expression" dxfId="8" priority="5">
       <formula>F7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>F7=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>F7=-1</formula>
     </cfRule>
     <cfRule type="iconSet" priority="22">
@@ -2914,13 +3194,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G18:G30">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>G18=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>G18=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>G18=-1</formula>
     </cfRule>
     <cfRule type="iconSet" priority="4">
@@ -2952,7 +3232,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Status icons in this column are automatically updated based on Done column value &amp; comparing Due Dates. Dates beyond the due date &amp; just before the due date are noted for emphasis" sqref="F6" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:G5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter idea details in cells at right. Enter Goal and Objective below. Enter tasks in Tasks table below" sqref="B2:C3" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E101" xr:uid="{00000000-0002-0000-0000-000015000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E115" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"Yes, No, Pending"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Add deadlines, responsibilities, restructured task
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebiru\code\Informatik-2.Jahr\IPT6.1\IPT6.1-Productivity-Game\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB782D3F-E376-418C-9671-95F74E234145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC07210-95A5-4319-8466-C771B81783F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4785" yWindow="-21600" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Idea Planner" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
   <definedNames>
     <definedName name="ColumnTitle1">Tasks[[#Headers],[ Task Status Indicator]]</definedName>
     <definedName name="ColumnTitleRegion1..G5.1">'Idea Planner'!$B$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Idea Planner'!$6:$6</definedName>
     <definedName name="PlanDueDate">'Idea Planner'!$E$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Idea Planner'!$6:$6</definedName>
     <definedName name="RowTitleRegion1..E3">'Idea Planner'!$D$2</definedName>
     <definedName name="RowTitleRegion2..G3">'Idea Planner'!$F$2</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -76,9 +76,6 @@
     <t>Status Icon</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -115,15 +112,6 @@
     <t>Wichtige Use-Cases beschreiben </t>
   </si>
   <si>
-    <t>Entitäten definieren</t>
-  </si>
-  <si>
-    <t>ER-Modell erstellen</t>
-  </si>
-  <si>
-    <t>Relationales Datenbankmodell erstellen</t>
-  </si>
-  <si>
     <t>Klassen definieren passend zur DB</t>
   </si>
   <si>
@@ -139,9 +127,6 @@
     <t>Zwecks- und Funktionsdefinition</t>
   </si>
   <si>
-    <t>Navigations bestimmen</t>
-  </si>
-  <si>
     <t>Benutzerabläufe festlegen</t>
   </si>
   <si>
@@ -340,9 +325,6 @@
     <t>2.3: Mockup-Erstellung</t>
   </si>
   <si>
-    <t>2.4: Datenmodell (DB)</t>
-  </si>
-  <si>
     <t>3.2: Authentifizierung</t>
   </si>
   <si>
@@ -473,6 +455,39 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>Webapplikation, Produktivität, Gamification</t>
+  </si>
+  <si>
+    <t>Responsibility</t>
+  </si>
+  <si>
+    <t>Sanjivan</t>
+  </si>
+  <si>
+    <t>Projektplan bestimmen</t>
+  </si>
+  <si>
+    <t>Egor</t>
+  </si>
+  <si>
+    <t>Sanjivan &amp; Egor</t>
+  </si>
+  <si>
+    <t>Navigation bestimmen</t>
+  </si>
+  <si>
+    <t>Create Scipt schreiben</t>
+  </si>
+  <si>
+    <t>Insert Script schreiben</t>
+  </si>
+  <si>
+    <t>Programmability Script schreiben</t>
+  </si>
+  <si>
+    <t>Beim Projekt handelt es sich um eine Web basierte Anwendung, welche die Produktivität des Benutzers fördern soll. Dies wird mit einem Spielerischem Ansatz erreicht (Gamification). Die Website soll Nutzern ermöglichen Tasks zu verwalten und abzuarbeiten, gleichzeitig aber den Nutzern zu motivieren die Task zu erledigen. Dafür werden Elemente der Spielebranche benutzt wie XP, Level, Streaks, welche die Arbeit messbar macht und motivierend wirkt.</t>
   </si>
 </sst>
 </file>
@@ -822,26 +837,26 @@
     </xf>
   </cellXfs>
   <cellStyles count="20">
-    <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Center aligned" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Comma" xfId="10" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="11" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="12" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="13" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Dezimal [0]" xfId="11" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Due Date" xfId="18" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Explanatory Text" xfId="7" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="14" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="7" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="10" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Plan Due Date" xfId="8" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Prozent" xfId="14" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Status Icon Text" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Task Indicator" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="15" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Währung" xfId="12" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Währung [0]" xfId="13" builtinId="7" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1037,7 +1052,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status Icon" dataCellStyle="Status Icon Text">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes" dataDxfId="6">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Responsibility" dataDxfId="6">
       <calculatedColumnFormula>IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1319,27 +1334,27 @@
   </sheetPr>
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.6328125" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="1" customWidth="1"/>
-    <col min="3" max="3" width="42.6328125" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="43.36328125" customWidth="1"/>
-    <col min="8" max="8" width="2.6328125" customWidth="1"/>
+    <col min="7" max="7" width="43.42578125" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
     </row>
-    <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
@@ -1348,16 +1363,16 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" s="5">
         <v>46185</v>
@@ -1366,10 +1381,10 @@
         <v>2</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="35" t="s">
         <v>3</v>
       </c>
@@ -1381,15 +1396,19 @@
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
-    <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="36"/>
+    <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="E5" s="36" t="s">
+        <v>137</v>
+      </c>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
-    <row r="6" spans="2:7" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1406,16 +1425,16 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C7" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
@@ -1423,442 +1442,497 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
       </c>
-      <c r="G7" s="26" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G7" s="26"/>
+    </row>
+    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="7">
         <v>46063</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F8" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G8" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" s="7">
         <v>46063</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F9" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G9" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D10" s="7">
         <v>46063</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F10" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
-      <c r="G10" s="27"/>
-    </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="19"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="11">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="12">
-        <v>46078</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="11">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
-      </c>
-      <c r="G12" s="27"/>
-    </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G10" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>140</v>
+      </c>
+      <c r="D11" s="7">
+        <v>46063</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" s="9">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D13" s="12">
         <v>46078</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F13" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G13" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" s="12">
         <v>46078</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G14" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D15" s="12">
         <v>46078</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G15" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D16" s="12">
         <v>46078</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F16" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="23"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G17" s="29"/>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="11">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="12">
+      <c r="G16" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="12">
         <v>46078</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="11">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
-      </c>
-      <c r="G18" s="11"/>
-    </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="23"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D19" s="12">
         <v>46078</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F19" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G19" s="11"/>
-    </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G19" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D20" s="12">
         <v>46078</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G20" s="11"/>
-    </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="23"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="25" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G21" s="25"/>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G20" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C22" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D22" s="12">
         <v>46078</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F22" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D23" s="12">
         <v>46078</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F23" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G23" s="11"/>
-    </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="25" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G24" s="25"/>
-    </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G23" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G24" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="D25" s="12">
         <v>46078</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G25" s="11"/>
-    </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G25" s="27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="C26" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="17" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G26" s="17"/>
-    </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="C26" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G26" s="25"/>
+    </row>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C27" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G27" s="11"/>
-    </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G27" s="30" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G28" s="11"/>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+      <c r="D28" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
-      <c r="C29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="12"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G29" s="11"/>
-    </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="C29" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="23"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G29" s="25"/>
+    </row>
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C30" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G30" s="11"/>
-    </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+      <c r="D30" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C31" s="14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="32"/>
@@ -1866,402 +1940,525 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
       </c>
-      <c r="G31" s="26"/>
-    </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C32" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>26</v>
+      </c>
+      <c r="D33" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>143</v>
+      </c>
+      <c r="D34" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F35" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="31"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="17" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G36" s="26"/>
+    </row>
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>28</v>
+      </c>
+      <c r="D37" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G37" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>29</v>
+      </c>
+      <c r="D38" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G38" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G39" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" s="31"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="17" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G40" s="26"/>
+    </row>
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>31</v>
+      </c>
+      <c r="D41" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G41" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>32</v>
+      </c>
+      <c r="D42" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F42" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C43" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G32" s="27"/>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C33" t="s">
+      <c r="D43" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E43" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C44" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G33" s="27"/>
-    </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C34" t="s">
+      <c r="D44" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F44" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G44" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C45" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G34" s="27"/>
-    </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="17" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G35" s="26"/>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C36" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="12"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G36" s="27"/>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C37" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G37" s="27"/>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C39" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G39" s="27"/>
-    </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="12"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D41" s="31"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="17" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G41" s="26"/>
-    </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C42" t="s">
-        <v>41</v>
-      </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G42" s="27"/>
-    </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B43" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C43" t="s">
-        <v>42</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G43" s="27"/>
-    </row>
-    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C44" t="s">
+      <c r="D45" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G45" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="11" t="str">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v/>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" s="23"/>
+      <c r="E46" s="24"/>
+      <c r="F46" s="25" t="str">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v/>
+      </c>
+      <c r="G46" s="29"/>
+    </row>
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C47" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G44" s="27" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C45" t="s">
+      <c r="D47" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F47" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G47" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>144</v>
+      </c>
+      <c r="D48" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E48" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F48" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G48" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>145</v>
+      </c>
+      <c r="D49" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E50" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G50" s="27" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C51" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="12"/>
-      <c r="E45" s="13"/>
-      <c r="F45" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G45" s="27"/>
-    </row>
-    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C46" t="s">
+      <c r="D51" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E51" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F51" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G51" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C52" t="s">
         <v>45</v>
       </c>
-      <c r="D46" s="12"/>
-      <c r="E46" s="13"/>
-      <c r="F46" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G46" s="27"/>
-    </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C47" t="s">
+      <c r="D52" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E52" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G52" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C53" t="s">
         <v>46</v>
       </c>
-      <c r="D47" s="12"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G47" s="27"/>
-    </row>
-    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C48" t="s">
+      <c r="D53" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E53" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G53" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C54" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="12"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G48" s="27"/>
-    </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C49" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="23"/>
-      <c r="E49" s="24"/>
-      <c r="F49" s="25" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G49" s="29"/>
-    </row>
-    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C50" t="s">
+      <c r="D54" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E54" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G54" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C55" t="s">
         <v>48</v>
       </c>
-      <c r="D50" s="12"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G50" s="27"/>
-    </row>
-    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B51" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C51" t="s">
-        <v>49</v>
-      </c>
-      <c r="D51" s="12"/>
-      <c r="E51" s="13"/>
-      <c r="F51" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G51" s="27"/>
-    </row>
-    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B52" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C52" t="s">
-        <v>50</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="13"/>
-      <c r="F52" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G52" s="27"/>
-    </row>
-    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B53" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C53" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="12"/>
-      <c r="E53" s="13"/>
-      <c r="F53" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G53" s="27"/>
-    </row>
-    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C54" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="12"/>
-      <c r="E54" s="13"/>
-      <c r="F54" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G54" s="27"/>
-    </row>
-    <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55" s="12"/>
-      <c r="E55" s="13"/>
-      <c r="F55" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G55" s="27"/>
-    </row>
-    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D55" s="12">
+        <v>46078</v>
+      </c>
+      <c r="E55" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G55" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C56" s="22" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D56" s="23"/>
       <c r="E56" s="24"/>
@@ -2271,13 +2468,13 @@
       </c>
       <c r="G56" s="29"/>
     </row>
-    <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C57" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="13"/>
@@ -2287,13 +2484,13 @@
       </c>
       <c r="G57" s="27"/>
     </row>
-    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
@@ -2303,13 +2500,13 @@
       </c>
       <c r="G58" s="27"/>
     </row>
-    <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C59" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="13"/>
@@ -2319,13 +2516,13 @@
       </c>
       <c r="G59" s="27"/>
     </row>
-    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13"/>
@@ -2335,13 +2532,13 @@
       </c>
       <c r="G60" s="27"/>
     </row>
-    <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C61" s="22" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="D61" s="23"/>
       <c r="E61" s="24"/>
@@ -2351,13 +2548,13 @@
       </c>
       <c r="G61" s="29"/>
     </row>
-    <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C62" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
@@ -2367,13 +2564,13 @@
       </c>
       <c r="G62" s="27"/>
     </row>
-    <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C63" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="13"/>
@@ -2383,13 +2580,13 @@
       </c>
       <c r="G63" s="27"/>
     </row>
-    <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B64" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C64" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="13"/>
@@ -2399,13 +2596,13 @@
       </c>
       <c r="G64" s="27"/>
     </row>
-    <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C65" s="22" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D65" s="23"/>
       <c r="E65" s="24"/>
@@ -2415,13 +2612,13 @@
       </c>
       <c r="G65" s="29"/>
     </row>
-    <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13"/>
@@ -2431,13 +2628,13 @@
       </c>
       <c r="G66" s="27"/>
     </row>
-    <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C67" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="13"/>
@@ -2447,13 +2644,13 @@
       </c>
       <c r="G67" s="27"/>
     </row>
-    <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="13"/>
@@ -2463,13 +2660,13 @@
       </c>
       <c r="G68" s="27"/>
     </row>
-    <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B69" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C69" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="13"/>
@@ -2479,13 +2676,13 @@
       </c>
       <c r="G69" s="27"/>
     </row>
-    <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C70" s="22" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D70" s="23"/>
       <c r="E70" s="24"/>
@@ -2495,13 +2692,13 @@
       </c>
       <c r="G70" s="29"/>
     </row>
-    <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C71" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="13"/>
@@ -2511,13 +2708,13 @@
       </c>
       <c r="G71" s="27"/>
     </row>
-    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C72" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="13"/>
@@ -2527,13 +2724,13 @@
       </c>
       <c r="G72" s="27"/>
     </row>
-    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B73" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C73" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="13"/>
@@ -2543,13 +2740,13 @@
       </c>
       <c r="G73" s="27"/>
     </row>
-    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B74" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C74" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="13"/>
@@ -2559,13 +2756,13 @@
       </c>
       <c r="G74" s="27"/>
     </row>
-    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B75" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C75" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="13"/>
@@ -2575,13 +2772,13 @@
       </c>
       <c r="G75" s="27"/>
     </row>
-    <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C76" s="22" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D76" s="23"/>
       <c r="E76" s="24"/>
@@ -2591,13 +2788,13 @@
       </c>
       <c r="G76" s="29"/>
     </row>
-    <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C77" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="13"/>
@@ -2607,13 +2804,13 @@
       </c>
       <c r="G77" s="27"/>
     </row>
-    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C78" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="13"/>
@@ -2623,13 +2820,13 @@
       </c>
       <c r="G78" s="27"/>
     </row>
-    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B79" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C79" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="13"/>
@@ -2639,13 +2836,13 @@
       </c>
       <c r="G79" s="27"/>
     </row>
-    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B80" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C80" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="13"/>
@@ -2655,13 +2852,13 @@
       </c>
       <c r="G80" s="27"/>
     </row>
-    <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C81" s="22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="24"/>
@@ -2671,13 +2868,13 @@
       </c>
       <c r="G81" s="29"/>
     </row>
-    <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B82" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="13"/>
@@ -2687,13 +2884,13 @@
       </c>
       <c r="G82" s="27"/>
     </row>
-    <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C83" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13"/>
@@ -2703,13 +2900,13 @@
       </c>
       <c r="G83" s="27"/>
     </row>
-    <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C84" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="13"/>
@@ -2719,13 +2916,13 @@
       </c>
       <c r="G84" s="27"/>
     </row>
-    <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C85" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D85" s="12"/>
       <c r="E85" s="13"/>
@@ -2735,13 +2932,13 @@
       </c>
       <c r="G85" s="27"/>
     </row>
-    <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C86" s="22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D86" s="23"/>
       <c r="E86" s="24"/>
@@ -2751,13 +2948,13 @@
       </c>
       <c r="G86" s="29"/>
     </row>
-    <row r="87" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B87" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C87" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="13"/>
@@ -2767,13 +2964,13 @@
       </c>
       <c r="G87" s="27"/>
     </row>
-    <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D88" s="12"/>
       <c r="E88" s="13"/>
@@ -2783,13 +2980,13 @@
       </c>
       <c r="G88" s="27"/>
     </row>
-    <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C89" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="13"/>
@@ -2799,13 +2996,13 @@
       </c>
       <c r="G89" s="27"/>
     </row>
-    <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C90" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D90" s="12"/>
       <c r="E90" s="13"/>
@@ -2815,13 +3012,13 @@
       </c>
       <c r="G90" s="27"/>
     </row>
-    <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="13"/>
@@ -2831,13 +3028,13 @@
       </c>
       <c r="G91" s="27"/>
     </row>
-    <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C92" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="13"/>
@@ -2847,13 +3044,13 @@
       </c>
       <c r="G92" s="27"/>
     </row>
-    <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C93" s="22" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D93" s="23"/>
       <c r="E93" s="24"/>
@@ -2863,13 +3060,13 @@
       </c>
       <c r="G93" s="29"/>
     </row>
-    <row r="94" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B94" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C94" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="13"/>
@@ -2879,13 +3076,13 @@
       </c>
       <c r="G94" s="27"/>
     </row>
-    <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C95" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="13"/>
@@ -2895,13 +3092,13 @@
       </c>
       <c r="G95" s="27"/>
     </row>
-    <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C96" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="13"/>
@@ -2911,13 +3108,13 @@
       </c>
       <c r="G96" s="27"/>
     </row>
-    <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C97" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="13"/>
@@ -2927,13 +3124,13 @@
       </c>
       <c r="G97" s="27"/>
     </row>
-    <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C98" s="22" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D98" s="23"/>
       <c r="E98" s="24"/>
@@ -2943,13 +3140,13 @@
       </c>
       <c r="G98" s="29"/>
     </row>
-    <row r="99" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C99" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D99" s="12"/>
       <c r="E99" s="13"/>
@@ -2959,13 +3156,13 @@
       </c>
       <c r="G99" s="27"/>
     </row>
-    <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C100" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="13"/>
@@ -2975,13 +3172,13 @@
       </c>
       <c r="G100" s="27"/>
     </row>
-    <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C101" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="13"/>
@@ -2991,13 +3188,13 @@
       </c>
       <c r="G101" s="27"/>
     </row>
-    <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C102" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="13"/>
@@ -3007,13 +3204,13 @@
       </c>
       <c r="G102" s="27"/>
     </row>
-    <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C103" s="22" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D103" s="23"/>
       <c r="E103" s="24"/>
@@ -3023,13 +3220,13 @@
       </c>
       <c r="G103" s="29"/>
     </row>
-    <row r="104" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C104" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="13"/>
@@ -3039,13 +3236,13 @@
       </c>
       <c r="G104" s="27"/>
     </row>
-    <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C105" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D105" s="12"/>
       <c r="E105" s="13"/>
@@ -3055,13 +3252,13 @@
       </c>
       <c r="G105" s="27"/>
     </row>
-    <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C106" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D106" s="12"/>
       <c r="E106" s="13"/>
@@ -3071,13 +3268,13 @@
       </c>
       <c r="G106" s="27"/>
     </row>
-    <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C107" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D107" s="12"/>
       <c r="E107" s="13"/>
@@ -3087,13 +3284,13 @@
       </c>
       <c r="G107" s="27"/>
     </row>
-    <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C108" s="22" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D108" s="23"/>
       <c r="E108" s="24"/>
@@ -3103,13 +3300,13 @@
       </c>
       <c r="G108" s="29"/>
     </row>
-    <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C109" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D109" s="12"/>
       <c r="E109" s="13"/>
@@ -3119,13 +3316,13 @@
       </c>
       <c r="G109" s="27"/>
     </row>
-    <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C110" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="13"/>
@@ -3135,13 +3332,13 @@
       </c>
       <c r="G110" s="27"/>
     </row>
-    <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C111" s="22" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D111" s="23"/>
       <c r="E111" s="24"/>
@@ -3151,13 +3348,13 @@
       </c>
       <c r="G111" s="29"/>
     </row>
-    <row r="112" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B112" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C112" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D112" s="12"/>
       <c r="E112" s="13"/>
@@ -3167,13 +3364,13 @@
       </c>
       <c r="G112" s="27"/>
     </row>
-    <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C113" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D113" s="12"/>
       <c r="E113" s="13"/>
@@ -3183,13 +3380,13 @@
       </c>
       <c r="G113" s="27"/>
     </row>
-    <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C114" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D114" s="12"/>
       <c r="E114" s="13"/>
@@ -3199,13 +3396,13 @@
       </c>
       <c r="G114" s="27"/>
     </row>
-    <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C115" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D115" s="12"/>
       <c r="E115" s="13"/>
@@ -3215,13 +3412,13 @@
       </c>
       <c r="G115" s="27"/>
     </row>
-    <row r="116" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C116" s="22" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D116" s="23"/>
       <c r="E116" s="24"/>
@@ -3231,13 +3428,13 @@
       </c>
       <c r="G116" s="29"/>
     </row>
-    <row r="117" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C117" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D117" s="12"/>
       <c r="E117" s="13"/>
@@ -3247,13 +3444,13 @@
       </c>
       <c r="G117" s="27"/>
     </row>
-    <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C118" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D118" s="12"/>
       <c r="E118" s="13"/>
@@ -3263,13 +3460,13 @@
       </c>
       <c r="G118" s="27"/>
     </row>
-    <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C119" s="22" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D119" s="23"/>
       <c r="E119" s="24"/>
@@ -3279,13 +3476,13 @@
       </c>
       <c r="G119" s="29"/>
     </row>
-    <row r="120" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C120" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D120" s="12"/>
       <c r="E120" s="13"/>
@@ -3295,13 +3492,13 @@
       </c>
       <c r="G120" s="27"/>
     </row>
-    <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C121" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D121" s="12"/>
       <c r="E121" s="13"/>
@@ -3311,13 +3508,13 @@
       </c>
       <c r="G121" s="27"/>
     </row>
-    <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C122" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D122" s="12"/>
       <c r="E122" s="13"/>
@@ -3327,13 +3524,13 @@
       </c>
       <c r="G122" s="27"/>
     </row>
-    <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C123" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D123" s="12"/>
       <c r="E123" s="13"/>
@@ -3343,13 +3540,13 @@
       </c>
       <c r="G123" s="27"/>
     </row>
-    <row r="124" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C124" s="22" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D124" s="23"/>
       <c r="E124" s="24"/>
@@ -3359,13 +3556,13 @@
       </c>
       <c r="G124" s="29"/>
     </row>
-    <row r="125" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C125" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D125" s="12"/>
       <c r="E125" s="13"/>
@@ -3375,13 +3572,13 @@
       </c>
       <c r="G125" s="27"/>
     </row>
-    <row r="126" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C126" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D126" s="12"/>
       <c r="E126" s="13"/>
@@ -3391,13 +3588,13 @@
       </c>
       <c r="G126" s="27"/>
     </row>
-    <row r="127" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C127" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D127" s="12"/>
       <c r="E127" s="13"/>
@@ -3407,13 +3604,13 @@
       </c>
       <c r="G127" s="27"/>
     </row>
-    <row r="128" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C128" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D128" s="12"/>
       <c r="E128" s="13"/>
@@ -3423,13 +3620,13 @@
       </c>
       <c r="G128" s="27"/>
     </row>
-    <row r="129" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C129" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D129" s="12"/>
       <c r="E129" s="13"/>
@@ -3439,13 +3636,13 @@
       </c>
       <c r="G129" s="27"/>
     </row>
-    <row r="130" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C130" s="22" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="D130" s="23"/>
       <c r="E130" s="24"/>
@@ -3455,13 +3652,13 @@
       </c>
       <c r="G130" s="29"/>
     </row>
-    <row r="131" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C131" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D131" s="12"/>
       <c r="E131" s="13"/>
@@ -3471,13 +3668,13 @@
       </c>
       <c r="G131" s="27"/>
     </row>
-    <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C132" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D132" s="12"/>
       <c r="E132" s="13"/>
@@ -3487,13 +3684,13 @@
       </c>
       <c r="G132" s="27"/>
     </row>
-    <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
       </c>
       <c r="C133" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D133" s="12"/>
       <c r="E133" s="13"/>
@@ -3524,33 +3721,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F133">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>F7=1</formula>
+  <conditionalFormatting sqref="G26:G35">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>G26=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>F7=0</formula>
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>G26=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
-      <formula>F7=-1</formula>
-    </cfRule>
-    <cfRule type="iconSet" priority="22">
-      <iconSet iconSet="3Symbols2">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G18:G30">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>G18=1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>G18=0</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>G18=-1</formula>
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>G26=-1</formula>
     </cfRule>
     <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols2">
@@ -3560,27 +3739,46 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations xWindow="1660" yWindow="543" count="21">
+  <conditionalFormatting sqref="F7:F133">
+    <cfRule type="expression" dxfId="2" priority="25">
+      <formula>F7=1</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="26">
+      <formula>F7=0</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="27">
+      <formula>F7=-1</formula>
+    </cfRule>
+    <cfRule type="iconSet" priority="28">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations xWindow="1660" yWindow="543" count="20">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create an Idea Planner in this worksheet. Set a Goal and an Objective, and enter task details in the Tasks table" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Image is in this cell. Title of this worksheet is in cell below" sqref="B1" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Topic in cell at right" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Topic in this cell" sqref="E2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in cell at right" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Keywords in cell at right" sqref="F2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Plan Due Date in cell at right" sqref="D3" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Plan Due Date in this cell" sqref="E3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in cell at right" sqref="F3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Name in this cell" sqref="G3" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Goal in cell below" sqref="B4:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in cell below" sqref="E4:G4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in cell below" sqref="E4:F4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Goal in this cell" sqref="B5:D5" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This column is automatically updated and indicates status based on column F" sqref="B6" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Tasks in this column under this heading" sqref="C6" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Due Date in this column under this heading" sqref="D6" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Notes in this column under this heading" sqref="G6" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select task completion status in this column. Press ALT+DOWN ARROW to open the drop-down list, ENTER to make selection. An icon representing this status is in the column at right" sqref="E6" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Status icons in this column are automatically updated based on Done column value &amp; comparing Due Dates. Dates beyond the due date &amp; just before the due date are noted for emphasis" sqref="F6" xr:uid="{00000000-0002-0000-0000-000012000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:G5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Objective in this cell" sqref="E5:F5" xr:uid="{00000000-0002-0000-0000-000013000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell. Enter idea details in cells at right. Enter Goal and Objective below. Enter tasks in Tasks table below" sqref="B2:C3" xr:uid="{00000000-0002-0000-0000-000014000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576" xr:uid="{482F76EC-3095-4ECD-80A0-E3C86F6A9FD3}">
+      <formula1>"Sanjivan,Egor,Sanjivan &amp; Egor, Unbestimmt"</formula1>
+    </dataValidation>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Select an option from the list. Press Cancel then ALT+DOWN ARROW to open the drop-down list, then ENTER to make selection" sqref="E7:E133" xr:uid="{00000000-0002-0000-0000-000015000000}">
       <formula1>"Yes, No, Pending"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Update Projektplan responsibilities and due dates
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC07210-95A5-4319-8466-C771B81783F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865AD914-A168-40C0-A683-1429F798895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Idea Planner" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -448,9 +448,6 @@
     <t>Github Actions vorbereiten</t>
   </si>
   <si>
-    <t>Projekten builden</t>
-  </si>
-  <si>
     <t>Projekt veröffentlichen</t>
   </si>
   <si>
@@ -488,6 +485,9 @@
   </si>
   <si>
     <t>Beim Projekt handelt es sich um eine Web basierte Anwendung, welche die Produktivität des Benutzers fördern soll. Dies wird mit einem Spielerischem Ansatz erreicht (Gamification). Die Website soll Nutzern ermöglichen Tasks zu verwalten und abzuarbeiten, gleichzeitig aber den Nutzern zu motivieren die Task zu erledigen. Dafür werden Elemente der Spielebranche benutzt wie XP, Level, Streaks, welche die Arbeit messbar macht und motivierend wirkt.</t>
+  </si>
+  <si>
+    <t>Projekt builden</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1334,8 @@
   </sheetPr>
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1398,12 +1398,12 @@
     </row>
     <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
       <c r="E5" s="36" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
@@ -1425,7 +1425,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1456,14 +1456,14 @@
         <v>46063</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F8" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1478,14 +1478,14 @@
         <v>46063</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F9" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,14 +1500,14 @@
         <v>46063</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F10" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1516,20 +1516,20 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D11" s="7">
         <v>46063</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F11" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1557,7 +1557,7 @@
         <v>17</v>
       </c>
       <c r="D13" s="12">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="E13" s="13" t="s">
         <v>10</v>
@@ -1567,7 +1567,7 @@
         <v>-1</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1579,7 +1579,7 @@
         <v>18</v>
       </c>
       <c r="D14" s="12">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>10</v>
@@ -1589,7 +1589,7 @@
         <v>-1</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,7 +1601,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="12">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>10</v>
@@ -1611,7 +1611,7 @@
         <v>-1</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1623,7 +1623,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="12">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>10</v>
@@ -1633,7 +1633,7 @@
         <v>-1</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1645,7 +1645,7 @@
         <v>21</v>
       </c>
       <c r="D17" s="12">
-        <v>46078</v>
+        <v>46079</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>10</v>
@@ -1655,7 +1655,7 @@
         <v>-1</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1683,7 +1683,7 @@
         <v>36</v>
       </c>
       <c r="D19" s="12">
-        <v>46078</v>
+        <v>46086</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>10</v>
@@ -1693,7 +1693,7 @@
         <v>-1</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1705,7 +1705,7 @@
         <v>37</v>
       </c>
       <c r="D20" s="12">
-        <v>46078</v>
+        <v>46086</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>10</v>
@@ -1715,7 +1715,7 @@
         <v>-1</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1727,7 @@
         <v>38</v>
       </c>
       <c r="D21" s="12">
-        <v>46078</v>
+        <v>46086</v>
       </c>
       <c r="E21" s="13" t="s">
         <v>10</v>
@@ -1737,7 +1737,7 @@
         <v>-1</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1749,7 +1749,7 @@
         <v>39</v>
       </c>
       <c r="D22" s="12">
-        <v>46078</v>
+        <v>46086</v>
       </c>
       <c r="E22" s="13" t="s">
         <v>10</v>
@@ -1759,7 +1759,7 @@
         <v>-1</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1771,7 +1771,7 @@
         <v>40</v>
       </c>
       <c r="D23" s="12">
-        <v>46078</v>
+        <v>46086</v>
       </c>
       <c r="E23" s="13" t="s">
         <v>10</v>
@@ -1781,7 +1781,7 @@
         <v>-1</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>41</v>
       </c>
       <c r="D24" s="12">
-        <v>46078</v>
+        <v>46093</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>10</v>
@@ -1803,7 +1803,7 @@
         <v>-1</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1815,7 +1815,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="12">
-        <v>46078</v>
+        <v>46093</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>10</v>
@@ -1825,7 +1825,7 @@
         <v>-1</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="D27" s="12">
-        <v>46078</v>
+        <v>46100</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>10</v>
@@ -1863,7 +1863,7 @@
         <v>-1</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1875,7 +1875,7 @@
         <v>23</v>
       </c>
       <c r="D28" s="12">
-        <v>46078</v>
+        <v>46100</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>10</v>
@@ -1885,7 +1885,7 @@
         <v>-1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1913,7 +1913,7 @@
         <v>24</v>
       </c>
       <c r="D30" s="12">
-        <v>46078</v>
+        <v>46107</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>10</v>
@@ -1923,7 +1923,7 @@
         <v>-1</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1951,7 +1951,7 @@
         <v>25</v>
       </c>
       <c r="D32" s="12">
-        <v>46078</v>
+        <v>46107</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>10</v>
@@ -1961,7 +1961,7 @@
         <v>-1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,7 +1973,7 @@
         <v>26</v>
       </c>
       <c r="D33" s="12">
-        <v>46078</v>
+        <v>46114</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>10</v>
@@ -1983,7 +1983,7 @@
         <v>-1</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1992,10 +1992,10 @@
         <v>-1</v>
       </c>
       <c r="C34" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D34" s="12">
-        <v>46078</v>
+        <v>46114</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>10</v>
@@ -2005,7 +2005,7 @@
         <v>-1</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
         <v>27</v>
       </c>
       <c r="D35" s="12">
-        <v>46078</v>
+        <v>46114</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>10</v>
@@ -2027,7 +2027,7 @@
         <v>-1</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2055,7 +2055,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>10</v>
@@ -2065,7 +2065,7 @@
         <v>-1</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,7 +2077,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>10</v>
@@ -2087,7 +2087,7 @@
         <v>-1</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>10</v>
@@ -2109,7 +2109,7 @@
         <v>-1</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2134,10 +2134,10 @@
         <v>-1</v>
       </c>
       <c r="C41" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D41" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>10</v>
@@ -2147,7 +2147,7 @@
         <v>-1</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2156,10 +2156,10 @@
         <v>-1</v>
       </c>
       <c r="C42" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D42" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>10</v>
@@ -2169,7 +2169,7 @@
         <v>-1</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2178,10 +2178,10 @@
         <v>-1</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D43" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>10</v>
@@ -2191,7 +2191,7 @@
         <v>-1</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2200,10 +2200,10 @@
         <v>-1</v>
       </c>
       <c r="C44" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D44" s="12">
-        <v>46078</v>
+        <v>46128</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>10</v>
@@ -2213,7 +2213,7 @@
         <v>-1</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2225,7 +2225,7 @@
         <v>35</v>
       </c>
       <c r="D45" s="12">
-        <v>46078</v>
+        <v>46128</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>10</v>
@@ -2235,7 +2235,7 @@
         <v>-1</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>43</v>
       </c>
       <c r="D47" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>10</v>
@@ -2273,7 +2273,7 @@
         <v>-1</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2282,10 +2282,10 @@
         <v>-1</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D48" s="12">
-        <v>46078</v>
+        <v>46121</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>10</v>
@@ -2295,7 +2295,7 @@
         <v>-1</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2304,10 +2304,10 @@
         <v>-1</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D49" s="12">
-        <v>46078</v>
+        <v>46128</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>10</v>
@@ -2317,7 +2317,7 @@
         <v>-1</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2326,10 +2326,10 @@
         <v>-1</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D50" s="12">
-        <v>46078</v>
+        <v>46128</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>10</v>
@@ -2339,7 +2339,7 @@
         <v>-1</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>44</v>
       </c>
       <c r="D51" s="12">
-        <v>46078</v>
+        <v>46135</v>
       </c>
       <c r="E51" s="13" t="s">
         <v>10</v>
@@ -2361,7 +2361,7 @@
         <v>-1</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2373,7 +2373,7 @@
         <v>45</v>
       </c>
       <c r="D52" s="12">
-        <v>46078</v>
+        <v>46135</v>
       </c>
       <c r="E52" s="13" t="s">
         <v>10</v>
@@ -2383,7 +2383,7 @@
         <v>-1</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>46</v>
       </c>
       <c r="D53" s="12">
-        <v>46078</v>
+        <v>46135</v>
       </c>
       <c r="E53" s="13" t="s">
         <v>10</v>
@@ -2405,7 +2405,7 @@
         <v>-1</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2417,7 +2417,7 @@
         <v>47</v>
       </c>
       <c r="D54" s="12">
-        <v>46078</v>
+        <v>46135</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>10</v>
@@ -2427,7 +2427,7 @@
         <v>-1</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>48</v>
       </c>
       <c r="D55" s="12">
-        <v>46078</v>
+        <v>46142</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>10</v>
@@ -2449,7 +2449,7 @@
         <v>-1</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,9 @@
         <v>49</v>
       </c>
       <c r="D57" s="12"/>
-      <c r="E57" s="13"/>
+      <c r="E57" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F57" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2493,7 +2495,9 @@
         <v>50</v>
       </c>
       <c r="D58" s="12"/>
-      <c r="E58" s="13"/>
+      <c r="E58" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F58" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2509,7 +2513,9 @@
         <v>51</v>
       </c>
       <c r="D59" s="12"/>
-      <c r="E59" s="13"/>
+      <c r="E59" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F59" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2525,7 +2531,9 @@
         <v>52</v>
       </c>
       <c r="D60" s="12"/>
-      <c r="E60" s="13"/>
+      <c r="E60" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F60" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2557,7 +2565,9 @@
         <v>53</v>
       </c>
       <c r="D62" s="12"/>
-      <c r="E62" s="13"/>
+      <c r="E62" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F62" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2573,7 +2583,9 @@
         <v>54</v>
       </c>
       <c r="D63" s="12"/>
-      <c r="E63" s="13"/>
+      <c r="E63" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F63" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2589,7 +2601,9 @@
         <v>55</v>
       </c>
       <c r="D64" s="12"/>
-      <c r="E64" s="13"/>
+      <c r="E64" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F64" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2621,7 +2635,9 @@
         <v>56</v>
       </c>
       <c r="D66" s="12"/>
-      <c r="E66" s="13"/>
+      <c r="E66" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F66" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2637,7 +2653,9 @@
         <v>57</v>
       </c>
       <c r="D67" s="12"/>
-      <c r="E67" s="13"/>
+      <c r="E67" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F67" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2653,7 +2671,9 @@
         <v>58</v>
       </c>
       <c r="D68" s="12"/>
-      <c r="E68" s="13"/>
+      <c r="E68" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F68" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2669,7 +2689,9 @@
         <v>59</v>
       </c>
       <c r="D69" s="12"/>
-      <c r="E69" s="13"/>
+      <c r="E69" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F69" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2701,7 +2723,9 @@
         <v>60</v>
       </c>
       <c r="D71" s="12"/>
-      <c r="E71" s="13"/>
+      <c r="E71" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F71" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2717,7 +2741,9 @@
         <v>61</v>
       </c>
       <c r="D72" s="12"/>
-      <c r="E72" s="13"/>
+      <c r="E72" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F72" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2733,7 +2759,9 @@
         <v>62</v>
       </c>
       <c r="D73" s="12"/>
-      <c r="E73" s="13"/>
+      <c r="E73" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F73" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2749,7 +2777,9 @@
         <v>63</v>
       </c>
       <c r="D74" s="12"/>
-      <c r="E74" s="13"/>
+      <c r="E74" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F74" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2765,7 +2795,9 @@
         <v>64</v>
       </c>
       <c r="D75" s="12"/>
-      <c r="E75" s="13"/>
+      <c r="E75" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F75" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2797,7 +2829,9 @@
         <v>65</v>
       </c>
       <c r="D77" s="12"/>
-      <c r="E77" s="13"/>
+      <c r="E77" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F77" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2813,7 +2847,9 @@
         <v>66</v>
       </c>
       <c r="D78" s="12"/>
-      <c r="E78" s="13"/>
+      <c r="E78" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F78" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2829,7 +2865,9 @@
         <v>67</v>
       </c>
       <c r="D79" s="12"/>
-      <c r="E79" s="13"/>
+      <c r="E79" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F79" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2845,7 +2883,9 @@
         <v>68</v>
       </c>
       <c r="D80" s="12"/>
-      <c r="E80" s="13"/>
+      <c r="E80" s="13" t="s">
+        <v>10</v>
+      </c>
       <c r="F80" s="11" t="str">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v/>
@@ -2869,66 +2909,82 @@
       <c r="G81" s="29"/>
     </row>
     <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B82" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C82" t="s">
         <v>69</v>
       </c>
-      <c r="D82" s="12"/>
-      <c r="E82" s="13"/>
-      <c r="F82" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D82" s="12">
+        <v>46114</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F82" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G82" s="27"/>
     </row>
     <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B83" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C83" t="s">
         <v>70</v>
       </c>
-      <c r="D83" s="12"/>
-      <c r="E83" s="13"/>
-      <c r="F83" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D83" s="12">
+        <v>46116</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F83" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G83" s="27"/>
     </row>
     <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B84" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C84" t="s">
         <v>71</v>
       </c>
-      <c r="D84" s="12"/>
-      <c r="E84" s="13"/>
-      <c r="F84" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D84" s="12">
+        <v>46116</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G84" s="27"/>
     </row>
     <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B85" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C85" t="s">
         <v>72</v>
       </c>
-      <c r="D85" s="12"/>
-      <c r="E85" s="13"/>
-      <c r="F85" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D85" s="12">
+        <v>46116</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G85" s="27"/>
     </row>
@@ -2949,98 +3005,122 @@
       <c r="G86" s="29"/>
     </row>
     <row r="87" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B87" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C87" t="s">
         <v>74</v>
       </c>
-      <c r="D87" s="12"/>
-      <c r="E87" s="13"/>
-      <c r="F87" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D87" s="12">
+        <v>46117</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G87" s="27"/>
     </row>
     <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B88" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C88" t="s">
         <v>75</v>
       </c>
-      <c r="D88" s="12"/>
-      <c r="E88" s="13"/>
-      <c r="F88" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D88" s="12">
+        <v>46119</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G88" s="27"/>
     </row>
     <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B89" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C89" t="s">
         <v>76</v>
       </c>
-      <c r="D89" s="12"/>
-      <c r="E89" s="13"/>
-      <c r="F89" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D89" s="12">
+        <v>46119</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G89" s="27"/>
     </row>
     <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B90" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C90" t="s">
         <v>77</v>
       </c>
-      <c r="D90" s="12"/>
-      <c r="E90" s="13"/>
-      <c r="F90" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D90" s="12">
+        <v>46119</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G90" s="27"/>
     </row>
     <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B91" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C91" t="s">
         <v>78</v>
       </c>
-      <c r="D91" s="12"/>
-      <c r="E91" s="13"/>
-      <c r="F91" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D91" s="12">
+        <v>46120</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G91" s="27"/>
     </row>
     <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B92" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C92" t="s">
         <v>79</v>
       </c>
-      <c r="D92" s="12"/>
-      <c r="E92" s="13"/>
-      <c r="F92" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D92" s="12">
+        <v>46120</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F92" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G92" s="27"/>
     </row>
@@ -3061,66 +3141,82 @@
       <c r="G93" s="29"/>
     </row>
     <row r="94" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B94" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C94" t="s">
         <v>81</v>
       </c>
-      <c r="D94" s="12"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D94" s="12">
+        <v>46123</v>
+      </c>
+      <c r="E94" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F94" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G94" s="27"/>
     </row>
     <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B95" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C95" t="s">
         <v>82</v>
       </c>
-      <c r="D95" s="12"/>
-      <c r="E95" s="13"/>
-      <c r="F95" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D95" s="12">
+        <v>46123</v>
+      </c>
+      <c r="E95" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F95" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G95" s="27"/>
     </row>
     <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B96" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C96" t="s">
         <v>83</v>
       </c>
-      <c r="D96" s="12"/>
-      <c r="E96" s="13"/>
-      <c r="F96" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D96" s="12">
+        <v>46123</v>
+      </c>
+      <c r="E96" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F96" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G96" s="27"/>
     </row>
     <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B97" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C97" t="s">
         <v>84</v>
       </c>
-      <c r="D97" s="12"/>
-      <c r="E97" s="13"/>
-      <c r="F97" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D97" s="12">
+        <v>46123</v>
+      </c>
+      <c r="E97" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G97" s="27"/>
     </row>
@@ -3141,66 +3237,82 @@
       <c r="G98" s="29"/>
     </row>
     <row r="99" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B99" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C99" t="s">
         <v>101</v>
       </c>
-      <c r="D99" s="12"/>
-      <c r="E99" s="13"/>
-      <c r="F99" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D99" s="12">
+        <v>46123</v>
+      </c>
+      <c r="E99" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G99" s="27"/>
     </row>
     <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B100" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C100" t="s">
         <v>102</v>
       </c>
-      <c r="D100" s="12"/>
-      <c r="E100" s="13"/>
-      <c r="F100" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D100" s="12">
+        <v>46125</v>
+      </c>
+      <c r="E100" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G100" s="27"/>
     </row>
     <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B101" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C101" t="s">
         <v>103</v>
       </c>
-      <c r="D101" s="12"/>
-      <c r="E101" s="13"/>
-      <c r="F101" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D101" s="12">
+        <v>46125</v>
+      </c>
+      <c r="E101" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G101" s="27"/>
     </row>
     <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B102" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C102" t="s">
         <v>104</v>
       </c>
-      <c r="D102" s="12"/>
-      <c r="E102" s="13"/>
-      <c r="F102" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D102" s="12">
+        <v>46125</v>
+      </c>
+      <c r="E102" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G102" s="27"/>
     </row>
@@ -3221,66 +3333,82 @@
       <c r="G103" s="29"/>
     </row>
     <row r="104" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B104" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C104" t="s">
         <v>106</v>
       </c>
-      <c r="D104" s="12"/>
-      <c r="E104" s="13"/>
-      <c r="F104" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D104" s="12">
+        <v>46128</v>
+      </c>
+      <c r="E104" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G104" s="27"/>
     </row>
     <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B105" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C105" t="s">
         <v>107</v>
       </c>
-      <c r="D105" s="12"/>
-      <c r="E105" s="13"/>
-      <c r="F105" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D105" s="12">
+        <v>46128</v>
+      </c>
+      <c r="E105" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G105" s="27"/>
     </row>
     <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B106" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C106" t="s">
         <v>108</v>
       </c>
-      <c r="D106" s="12"/>
-      <c r="E106" s="13"/>
-      <c r="F106" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D106" s="12">
+        <v>46128</v>
+      </c>
+      <c r="E106" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F106" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G106" s="27"/>
     </row>
     <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B107" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C107" t="s">
         <v>109</v>
       </c>
-      <c r="D107" s="12"/>
-      <c r="E107" s="13"/>
-      <c r="F107" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D107" s="12">
+        <v>46128</v>
+      </c>
+      <c r="E107" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G107" s="27"/>
     </row>
@@ -3301,34 +3429,42 @@
       <c r="G108" s="29"/>
     </row>
     <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B109" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C109" t="s">
         <v>111</v>
       </c>
-      <c r="D109" s="12"/>
-      <c r="E109" s="13"/>
-      <c r="F109" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D109" s="12">
+        <v>46133</v>
+      </c>
+      <c r="E109" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G109" s="27"/>
     </row>
     <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B110" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B110" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C110" t="s">
         <v>112</v>
       </c>
-      <c r="D110" s="12"/>
-      <c r="E110" s="13"/>
-      <c r="F110" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D110" s="12">
+        <v>46133</v>
+      </c>
+      <c r="E110" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G110" s="27"/>
     </row>
@@ -3349,66 +3485,82 @@
       <c r="G111" s="29"/>
     </row>
     <row r="112" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B112" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B112" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C112" t="s">
         <v>114</v>
       </c>
-      <c r="D112" s="12"/>
-      <c r="E112" s="13"/>
-      <c r="F112" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D112" s="12">
+        <v>46135</v>
+      </c>
+      <c r="E112" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G112" s="27"/>
     </row>
     <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B113" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C113" t="s">
         <v>115</v>
       </c>
-      <c r="D113" s="12"/>
-      <c r="E113" s="13"/>
-      <c r="F113" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D113" s="12">
+        <v>46142</v>
+      </c>
+      <c r="E113" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G113" s="27"/>
     </row>
     <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B114" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C114" t="s">
         <v>116</v>
       </c>
-      <c r="D114" s="12"/>
-      <c r="E114" s="13"/>
-      <c r="F114" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D114" s="12">
+        <v>46142</v>
+      </c>
+      <c r="E114" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G114" s="27"/>
     </row>
     <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B115" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C115" t="s">
         <v>117</v>
       </c>
-      <c r="D115" s="12"/>
-      <c r="E115" s="13"/>
-      <c r="F115" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D115" s="12">
+        <v>46142</v>
+      </c>
+      <c r="E115" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G115" s="27"/>
     </row>
@@ -3429,34 +3581,42 @@
       <c r="G116" s="29"/>
     </row>
     <row r="117" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B117" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B117" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C117" t="s">
         <v>119</v>
       </c>
-      <c r="D117" s="12"/>
-      <c r="E117" s="13"/>
-      <c r="F117" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D117" s="12">
+        <v>46156</v>
+      </c>
+      <c r="E117" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G117" s="27"/>
     </row>
     <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B118" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C118" t="s">
         <v>120</v>
       </c>
-      <c r="D118" s="12"/>
-      <c r="E118" s="13"/>
-      <c r="F118" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D118" s="12">
+        <v>46156</v>
+      </c>
+      <c r="E118" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G118" s="27"/>
     </row>
@@ -3477,66 +3637,82 @@
       <c r="G119" s="29"/>
     </row>
     <row r="120" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B120" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C120" t="s">
         <v>122</v>
       </c>
-      <c r="D120" s="12"/>
-      <c r="E120" s="13"/>
-      <c r="F120" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D120" s="12">
+        <v>46163</v>
+      </c>
+      <c r="E120" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F120" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G120" s="27"/>
     </row>
     <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B121" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B121" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C121" t="s">
         <v>123</v>
       </c>
-      <c r="D121" s="12"/>
-      <c r="E121" s="13"/>
-      <c r="F121" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D121" s="12">
+        <v>46170</v>
+      </c>
+      <c r="E121" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G121" s="27"/>
     </row>
     <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B122" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B122" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C122" t="s">
         <v>124</v>
       </c>
-      <c r="D122" s="12"/>
-      <c r="E122" s="13"/>
-      <c r="F122" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D122" s="12">
+        <v>46170</v>
+      </c>
+      <c r="E122" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G122" s="27"/>
     </row>
     <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B123" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B123" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C123" t="s">
         <v>125</v>
       </c>
-      <c r="D123" s="12"/>
-      <c r="E123" s="13"/>
-      <c r="F123" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D123" s="12">
+        <v>46170</v>
+      </c>
+      <c r="E123" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F123" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G123" s="27"/>
     </row>
@@ -3557,84 +3733,114 @@
       <c r="G124" s="29"/>
     </row>
     <row r="125" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B125" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B125" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C125" t="s">
         <v>127</v>
       </c>
-      <c r="D125" s="12"/>
-      <c r="E125" s="13"/>
-      <c r="F125" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G125" s="27"/>
+      <c r="D125" s="12">
+        <v>46177</v>
+      </c>
+      <c r="E125" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F125" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G125" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="126" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B126" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B126" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C126" t="s">
         <v>128</v>
       </c>
-      <c r="D126" s="12"/>
-      <c r="E126" s="13"/>
-      <c r="F126" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G126" s="27"/>
+      <c r="D126" s="12">
+        <v>46177</v>
+      </c>
+      <c r="E126" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F126" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G126" s="27" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="127" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B127" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B127" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C127" t="s">
         <v>129</v>
       </c>
-      <c r="D127" s="12"/>
-      <c r="E127" s="13"/>
-      <c r="F127" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G127" s="27"/>
+      <c r="D127" s="12">
+        <v>46177</v>
+      </c>
+      <c r="E127" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F127" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G127" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="128" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B128" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B128" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C128" t="s">
         <v>130</v>
       </c>
-      <c r="D128" s="12"/>
-      <c r="E128" s="13"/>
-      <c r="F128" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G128" s="27"/>
+      <c r="D128" s="12">
+        <v>46177</v>
+      </c>
+      <c r="E128" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F128" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G128" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="129" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B129" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B129" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C129" t="s">
         <v>131</v>
       </c>
-      <c r="D129" s="12"/>
-      <c r="E129" s="13"/>
-      <c r="F129" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G129" s="27"/>
+      <c r="D129" s="12">
+        <v>46177</v>
+      </c>
+      <c r="E129" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F129" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G129" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="130" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="11" t="str">
@@ -3653,50 +3859,62 @@
       <c r="G130" s="29"/>
     </row>
     <row r="131" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B131" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B131" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C131" t="s">
         <v>133</v>
       </c>
-      <c r="D131" s="12"/>
-      <c r="E131" s="13"/>
-      <c r="F131" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D131" s="12">
+        <v>46185</v>
+      </c>
+      <c r="E131" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F131" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G131" s="27"/>
     </row>
     <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B132" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B132" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C132" t="s">
+        <v>147</v>
+      </c>
+      <c r="D132" s="12">
+        <v>46185</v>
+      </c>
+      <c r="E132" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F132" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G132" s="27"/>
+    </row>
+    <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C133" t="s">
         <v>134</v>
       </c>
-      <c r="D132" s="12"/>
-      <c r="E132" s="13"/>
-      <c r="F132" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G132" s="27"/>
-    </row>
-    <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B133" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C133" t="s">
-        <v>135</v>
-      </c>
-      <c r="D133" s="12"/>
-      <c r="E133" s="13"/>
-      <c r="F133" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
+      <c r="D133" s="12">
+        <v>46185</v>
+      </c>
+      <c r="E133" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F133" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
       </c>
       <c r="G133" s="27"/>
     </row>
@@ -3721,17 +3939,17 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G35">
-    <cfRule type="expression" dxfId="5" priority="1">
-      <formula>G26=1</formula>
+  <conditionalFormatting sqref="F7:F133">
+    <cfRule type="expression" dxfId="5" priority="25">
+      <formula>F7=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
-      <formula>G26=0</formula>
+    <cfRule type="expression" dxfId="4" priority="26">
+      <formula>F7=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>G26=-1</formula>
+    <cfRule type="expression" dxfId="3" priority="27">
+      <formula>F7=-1</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="28">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
@@ -3739,17 +3957,17 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F133">
-    <cfRule type="expression" dxfId="2" priority="25">
-      <formula>F7=1</formula>
+  <conditionalFormatting sqref="G26:G35">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>G26=1</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="26">
-      <formula>F7=0</formula>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>G26=0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="27">
-      <formula>F7=-1</formula>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>G26=-1</formula>
     </cfRule>
-    <cfRule type="iconSet" priority="28">
+    <cfRule type="iconSet" priority="4">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Change due dates, justify responsibilities
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865AD914-A168-40C0-A683-1429F798895F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCB38FC-5291-4309-A704-BDFC6B412D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="148">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -1334,8 +1334,8 @@
   </sheetPr>
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1793,7 @@
         <v>41</v>
       </c>
       <c r="D24" s="12">
-        <v>46093</v>
+        <v>46086</v>
       </c>
       <c r="E24" s="13" t="s">
         <v>10</v>
@@ -1815,7 +1815,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="12">
-        <v>46093</v>
+        <v>46086</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>10</v>
@@ -1853,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="D27" s="12">
-        <v>46100</v>
+        <v>46093</v>
       </c>
       <c r="E27" s="13" t="s">
         <v>10</v>
@@ -1875,7 +1875,7 @@
         <v>23</v>
       </c>
       <c r="D28" s="12">
-        <v>46100</v>
+        <v>46093</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>10</v>
@@ -1913,7 +1913,7 @@
         <v>24</v>
       </c>
       <c r="D30" s="12">
-        <v>46107</v>
+        <v>46093</v>
       </c>
       <c r="E30" s="13" t="s">
         <v>10</v>
@@ -1951,7 +1951,7 @@
         <v>25</v>
       </c>
       <c r="D32" s="12">
-        <v>46107</v>
+        <v>46100</v>
       </c>
       <c r="E32" s="13" t="s">
         <v>10</v>
@@ -1973,7 +1973,7 @@
         <v>26</v>
       </c>
       <c r="D33" s="12">
-        <v>46114</v>
+        <v>46100</v>
       </c>
       <c r="E33" s="13" t="s">
         <v>10</v>
@@ -1995,7 +1995,7 @@
         <v>142</v>
       </c>
       <c r="D34" s="12">
-        <v>46114</v>
+        <v>46100</v>
       </c>
       <c r="E34" s="13" t="s">
         <v>10</v>
@@ -2017,7 +2017,7 @@
         <v>27</v>
       </c>
       <c r="D35" s="12">
-        <v>46114</v>
+        <v>46100</v>
       </c>
       <c r="E35" s="13" t="s">
         <v>10</v>
@@ -2055,7 +2055,7 @@
         <v>28</v>
       </c>
       <c r="D37" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>10</v>
@@ -2077,7 +2077,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E38" s="13" t="s">
         <v>10</v>
@@ -2099,7 +2099,7 @@
         <v>30</v>
       </c>
       <c r="D39" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>10</v>
@@ -2137,7 +2137,7 @@
         <v>32</v>
       </c>
       <c r="D41" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E41" s="13" t="s">
         <v>10</v>
@@ -2159,7 +2159,7 @@
         <v>33</v>
       </c>
       <c r="D42" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E42" s="13" t="s">
         <v>10</v>
@@ -2181,7 +2181,7 @@
         <v>34</v>
       </c>
       <c r="D43" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E43" s="13" t="s">
         <v>10</v>
@@ -2203,7 +2203,7 @@
         <v>31</v>
       </c>
       <c r="D44" s="12">
-        <v>46128</v>
+        <v>46112</v>
       </c>
       <c r="E44" s="13" t="s">
         <v>10</v>
@@ -2225,7 +2225,7 @@
         <v>35</v>
       </c>
       <c r="D45" s="12">
-        <v>46128</v>
+        <v>46112</v>
       </c>
       <c r="E45" s="13" t="s">
         <v>10</v>
@@ -2263,7 +2263,7 @@
         <v>43</v>
       </c>
       <c r="D47" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>10</v>
@@ -2285,7 +2285,7 @@
         <v>143</v>
       </c>
       <c r="D48" s="12">
-        <v>46121</v>
+        <v>46107</v>
       </c>
       <c r="E48" s="13" t="s">
         <v>10</v>
@@ -2307,7 +2307,7 @@
         <v>144</v>
       </c>
       <c r="D49" s="12">
-        <v>46128</v>
+        <v>46112</v>
       </c>
       <c r="E49" s="13" t="s">
         <v>10</v>
@@ -2329,7 +2329,7 @@
         <v>145</v>
       </c>
       <c r="D50" s="12">
-        <v>46128</v>
+        <v>46112</v>
       </c>
       <c r="E50" s="13" t="s">
         <v>10</v>
@@ -2926,7 +2926,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G82" s="27"/>
+      <c r="G82" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B83" s="11">
@@ -2946,7 +2948,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G83" s="27"/>
+      <c r="G83" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B84" s="11">
@@ -2966,7 +2970,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G84" s="27"/>
+      <c r="G84" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B85" s="11">
@@ -2986,7 +2992,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G85" s="27"/>
+      <c r="G85" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B86" s="11" t="str">
@@ -3022,7 +3030,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G87" s="27"/>
+      <c r="G87" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="11">
@@ -3042,7 +3052,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G88" s="27"/>
+      <c r="G88" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="11">
@@ -3062,7 +3074,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G89" s="27"/>
+      <c r="G89" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B90" s="11">
@@ -3082,7 +3096,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G90" s="27"/>
+      <c r="G90" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B91" s="11">
@@ -3102,7 +3118,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G91" s="27"/>
+      <c r="G91" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="11">
@@ -3122,7 +3140,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G92" s="27"/>
+      <c r="G92" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B93" s="11" t="str">
@@ -3158,7 +3178,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G94" s="27"/>
+      <c r="G94" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B95" s="11">
@@ -3178,7 +3200,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G95" s="27"/>
+      <c r="G95" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="11">
@@ -3198,7 +3222,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G96" s="27"/>
+      <c r="G96" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B97" s="11">
@@ -3218,7 +3244,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G97" s="27"/>
+      <c r="G97" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="11" t="str">
@@ -3254,7 +3282,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G99" s="27"/>
+      <c r="G99" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" s="11">
@@ -3274,7 +3304,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G100" s="27"/>
+      <c r="G100" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B101" s="11">
@@ -3294,7 +3326,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G101" s="27"/>
+      <c r="G101" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="11">
@@ -3314,7 +3348,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G102" s="27"/>
+      <c r="G102" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B103" s="11" t="str">
@@ -3350,7 +3386,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G104" s="27"/>
+      <c r="G104" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B105" s="11">
@@ -3370,7 +3408,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G105" s="27"/>
+      <c r="G105" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B106" s="11">
@@ -3390,7 +3430,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G106" s="27"/>
+      <c r="G106" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B107" s="11">
@@ -3410,7 +3452,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G107" s="27"/>
+      <c r="G107" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B108" s="11" t="str">
@@ -3446,7 +3490,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G109" s="27"/>
+      <c r="G109" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B110" s="11">
@@ -3466,7 +3512,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G110" s="27"/>
+      <c r="G110" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B111" s="11" t="str">
@@ -3502,7 +3550,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G112" s="27"/>
+      <c r="G112" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B113" s="11">
@@ -3522,7 +3572,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G113" s="27"/>
+      <c r="G113" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B114" s="11">
@@ -3542,7 +3594,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G114" s="27"/>
+      <c r="G114" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B115" s="11">
@@ -3562,7 +3616,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G115" s="27"/>
+      <c r="G115" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="116" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="11" t="str">
@@ -3598,7 +3654,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G117" s="27"/>
+      <c r="G117" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B118" s="11">
@@ -3618,7 +3676,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G118" s="27"/>
+      <c r="G118" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="11" t="str">
@@ -3654,7 +3714,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G120" s="27"/>
+      <c r="G120" s="27" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="11">
@@ -3674,7 +3736,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G121" s="27"/>
+      <c r="G121" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="11">
@@ -3694,7 +3758,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G122" s="27"/>
+      <c r="G122" s="27" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="11">
@@ -3714,7 +3780,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G123" s="27"/>
+      <c r="G123" s="27" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="124" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="11" t="str">
@@ -3876,7 +3944,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G131" s="27"/>
+      <c r="G131" s="27" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="11">
@@ -3896,7 +3966,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G132" s="27"/>
+      <c r="G132" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="11">
@@ -3916,7 +3988,9 @@
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>-1</v>
       </c>
-      <c r="G133" s="27"/>
+      <c r="G133" s="27" t="s">
+        <v>138</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
fill all deadlines & responsibilities phase 3-5
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCB38FC-5291-4309-A704-BDFC6B412D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A883F74D-4F2F-4145-870A-C83CB6069CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Idea Planner" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="148">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -223,9 +223,6 @@
     <t>XP als Event in der DB speichern (XPEvent)</t>
   </si>
   <si>
-    <t>Gesamt-XP pro User berechnen/abrufend</t>
-  </si>
-  <si>
     <t>Level Grenzen definieren</t>
   </si>
   <si>
@@ -488,6 +485,9 @@
   </si>
   <si>
     <t>Projekt builden</t>
+  </si>
+  <si>
+    <t>Gesamt-XP pro User berechnen/abrufen</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1334,8 @@
   </sheetPr>
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A42" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1398,12 +1398,12 @@
     </row>
     <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
       <c r="E5" s="36" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
@@ -1425,7 +1425,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1434,7 +1434,7 @@
         <v/>
       </c>
       <c r="C7" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
@@ -1456,14 +1456,14 @@
         <v>46063</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F8" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1478,14 +1478,14 @@
         <v>46063</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F9" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1500,14 +1500,14 @@
         <v>46063</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F10" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1516,20 +1516,20 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="7">
         <v>46063</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F11" s="9">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
         <v>1</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1538,7 +1538,7 @@
         <v/>
       </c>
       <c r="C12" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
@@ -1567,7 +1567,7 @@
         <v>-1</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,7 +1589,7 @@
         <v>-1</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1611,7 +1611,7 @@
         <v>-1</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1633,7 +1633,7 @@
         <v>-1</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1655,7 +1655,7 @@
         <v>-1</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1664,7 +1664,7 @@
         <v/>
       </c>
       <c r="C18" s="22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="23"/>
       <c r="E18" s="24"/>
@@ -1693,7 +1693,7 @@
         <v>-1</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1715,7 +1715,7 @@
         <v>-1</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1737,7 +1737,7 @@
         <v>-1</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1759,7 +1759,7 @@
         <v>-1</v>
       </c>
       <c r="G22" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,7 +1781,7 @@
         <v>-1</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1803,7 +1803,7 @@
         <v>-1</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1825,7 +1825,7 @@
         <v>-1</v>
       </c>
       <c r="G25" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
         <v/>
       </c>
       <c r="C26" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D26" s="23"/>
       <c r="E26" s="24"/>
@@ -1863,7 +1863,7 @@
         <v>-1</v>
       </c>
       <c r="G27" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1885,7 +1885,7 @@
         <v>-1</v>
       </c>
       <c r="G28" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v/>
       </c>
       <c r="C29" s="22" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D29" s="23"/>
       <c r="E29" s="24"/>
@@ -1923,7 +1923,7 @@
         <v>-1</v>
       </c>
       <c r="G30" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1932,7 +1932,7 @@
         <v/>
       </c>
       <c r="C31" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="32"/>
@@ -1961,7 +1961,7 @@
         <v>-1</v>
       </c>
       <c r="G32" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1983,7 +1983,7 @@
         <v>-1</v>
       </c>
       <c r="G33" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>-1</v>
       </c>
       <c r="C34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" s="12">
         <v>46100</v>
@@ -2005,7 +2005,7 @@
         <v>-1</v>
       </c>
       <c r="G34" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2027,7 +2027,7 @@
         <v>-1</v>
       </c>
       <c r="G35" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2036,7 +2036,7 @@
         <v/>
       </c>
       <c r="C36" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D36" s="31"/>
       <c r="E36" s="32"/>
@@ -2065,7 +2065,7 @@
         <v>-1</v>
       </c>
       <c r="G37" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>-1</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,7 +2109,7 @@
         <v>-1</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2118,7 +2118,7 @@
         <v/>
       </c>
       <c r="C40" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D40" s="31"/>
       <c r="E40" s="32"/>
@@ -2147,7 +2147,7 @@
         <v>-1</v>
       </c>
       <c r="G41" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2169,7 +2169,7 @@
         <v>-1</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>-1</v>
       </c>
       <c r="G43" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>-1</v>
       </c>
       <c r="G44" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2235,7 +2235,7 @@
         <v>-1</v>
       </c>
       <c r="G45" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v/>
       </c>
       <c r="C46" s="22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D46" s="23"/>
       <c r="E46" s="24"/>
@@ -2273,7 +2273,7 @@
         <v>-1</v>
       </c>
       <c r="G47" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2282,7 +2282,7 @@
         <v>-1</v>
       </c>
       <c r="C48" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D48" s="12">
         <v>46107</v>
@@ -2295,7 +2295,7 @@
         <v>-1</v>
       </c>
       <c r="G48" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
         <v>-1</v>
       </c>
       <c r="C49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D49" s="12">
         <v>46112</v>
@@ -2317,7 +2317,7 @@
         <v>-1</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2326,7 +2326,7 @@
         <v>-1</v>
       </c>
       <c r="C50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D50" s="12">
         <v>46112</v>
@@ -2339,7 +2339,7 @@
         <v>-1</v>
       </c>
       <c r="G50" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2361,7 +2361,7 @@
         <v>-1</v>
       </c>
       <c r="G51" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
         <v>-1</v>
       </c>
       <c r="G52" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2405,7 +2405,7 @@
         <v>-1</v>
       </c>
       <c r="G53" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2427,7 +2427,7 @@
         <v>-1</v>
       </c>
       <c r="G54" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>48</v>
       </c>
       <c r="D55" s="12">
-        <v>46142</v>
+        <v>46111</v>
       </c>
       <c r="E55" s="13" t="s">
         <v>10</v>
@@ -2449,7 +2449,7 @@
         <v>-1</v>
       </c>
       <c r="G55" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2458,7 +2458,7 @@
         <v/>
       </c>
       <c r="C56" s="22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" s="23"/>
       <c r="E56" s="24"/>
@@ -2469,76 +2469,92 @@
       <c r="G56" s="29"/>
     </row>
     <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B57" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C57" t="s">
         <v>49</v>
       </c>
-      <c r="D57" s="12"/>
+      <c r="D57" s="12">
+        <v>46111</v>
+      </c>
       <c r="E57" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G57" s="27"/>
+      <c r="F57" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B58" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C58" t="s">
         <v>50</v>
       </c>
-      <c r="D58" s="12"/>
+      <c r="D58" s="12">
+        <v>46111</v>
+      </c>
       <c r="E58" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G58" s="27"/>
+      <c r="F58" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G58" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B59" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C59" t="s">
         <v>51</v>
       </c>
-      <c r="D59" s="12"/>
+      <c r="D59" s="12">
+        <v>46111</v>
+      </c>
       <c r="E59" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F59" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G59" s="27"/>
+      <c r="F59" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B60" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C60" t="s">
         <v>52</v>
       </c>
-      <c r="D60" s="12"/>
+      <c r="D60" s="12">
+        <v>46111</v>
+      </c>
       <c r="E60" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F60" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G60" s="27"/>
+      <c r="F60" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G60" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="str">
@@ -2546,7 +2562,7 @@
         <v/>
       </c>
       <c r="C61" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D61" s="23"/>
       <c r="E61" s="24"/>
@@ -2557,58 +2573,70 @@
       <c r="G61" s="29"/>
     </row>
     <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B62" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C62" t="s">
         <v>53</v>
       </c>
-      <c r="D62" s="12"/>
+      <c r="D62" s="12">
+        <v>46111</v>
+      </c>
       <c r="E62" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G62" s="27"/>
+      <c r="F62" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G62" s="27" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B63" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C63" t="s">
         <v>54</v>
       </c>
-      <c r="D63" s="12"/>
+      <c r="D63" s="12">
+        <v>46111</v>
+      </c>
       <c r="E63" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G63" s="27"/>
+      <c r="F63" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G63" s="27" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B64" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C64" t="s">
         <v>55</v>
       </c>
-      <c r="D64" s="12"/>
+      <c r="D64" s="12">
+        <v>46111</v>
+      </c>
       <c r="E64" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G64" s="27"/>
+      <c r="F64" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G64" s="27" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="11" t="str">
@@ -2616,7 +2644,7 @@
         <v/>
       </c>
       <c r="C65" s="22" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D65" s="23"/>
       <c r="E65" s="24"/>
@@ -2627,76 +2655,92 @@
       <c r="G65" s="29"/>
     </row>
     <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B66" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C66" t="s">
         <v>56</v>
       </c>
-      <c r="D66" s="12"/>
+      <c r="D66" s="12">
+        <v>46114</v>
+      </c>
       <c r="E66" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F66" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G66" s="27"/>
+      <c r="F66" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G66" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B67" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C67" t="s">
         <v>57</v>
       </c>
-      <c r="D67" s="12"/>
+      <c r="D67" s="12">
+        <v>46114</v>
+      </c>
       <c r="E67" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F67" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G67" s="27"/>
+      <c r="F67" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G67" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B68" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C68" t="s">
         <v>58</v>
       </c>
-      <c r="D68" s="12"/>
+      <c r="D68" s="12">
+        <v>46114</v>
+      </c>
       <c r="E68" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F68" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G68" s="27"/>
+      <c r="F68" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G68" s="27" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B69" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C69" t="s">
-        <v>59</v>
-      </c>
-      <c r="D69" s="12"/>
+        <v>147</v>
+      </c>
+      <c r="D69" s="12">
+        <v>46114</v>
+      </c>
       <c r="E69" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F69" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G69" s="27"/>
+      <c r="F69" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G69" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B70" s="11" t="str">
@@ -2704,7 +2748,7 @@
         <v/>
       </c>
       <c r="C70" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D70" s="23"/>
       <c r="E70" s="24"/>
@@ -2715,94 +2759,114 @@
       <c r="G70" s="29"/>
     </row>
     <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B71" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" s="12">
+        <v>46114</v>
+      </c>
+      <c r="E71" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F71" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G71" s="27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C72" t="s">
         <v>60</v>
       </c>
-      <c r="D71" s="12"/>
-      <c r="E71" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G71" s="27"/>
-    </row>
-    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C72" t="s">
+      <c r="D72" s="12">
+        <v>46114</v>
+      </c>
+      <c r="E72" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G72" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C73" t="s">
         <v>61</v>
       </c>
-      <c r="D72" s="12"/>
-      <c r="E72" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F72" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G72" s="27"/>
-    </row>
-    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C73" t="s">
+      <c r="D73" s="12">
+        <v>46114</v>
+      </c>
+      <c r="E73" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G73" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C74" t="s">
         <v>62</v>
       </c>
-      <c r="D73" s="12"/>
-      <c r="E73" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G73" s="27"/>
-    </row>
-    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C74" t="s">
+      <c r="D74" s="12">
+        <v>46114</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G74" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C75" t="s">
         <v>63</v>
       </c>
-      <c r="D74" s="12"/>
-      <c r="E74" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F74" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G74" s="27"/>
-    </row>
-    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C75" t="s">
-        <v>64</v>
-      </c>
-      <c r="D75" s="12"/>
+      <c r="D75" s="12">
+        <v>46114</v>
+      </c>
       <c r="E75" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F75" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G75" s="27"/>
+      <c r="F75" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="11" t="str">
@@ -2810,7 +2874,7 @@
         <v/>
       </c>
       <c r="C76" s="22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D76" s="23"/>
       <c r="E76" s="24"/>
@@ -2821,76 +2885,92 @@
       <c r="G76" s="29"/>
     </row>
     <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
+      <c r="B77" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
       </c>
       <c r="C77" t="s">
+        <v>64</v>
+      </c>
+      <c r="D77" s="12">
+        <v>46116</v>
+      </c>
+      <c r="E77" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G77" s="27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C78" t="s">
         <v>65</v>
       </c>
-      <c r="D77" s="12"/>
-      <c r="E77" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G77" s="27"/>
-    </row>
-    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C78" t="s">
+      <c r="D78" s="12">
+        <v>46116</v>
+      </c>
+      <c r="E78" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G78" s="27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C79" t="s">
         <v>66</v>
       </c>
-      <c r="D78" s="12"/>
-      <c r="E78" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F78" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G78" s="27"/>
-    </row>
-    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C79" t="s">
+      <c r="D79" s="12">
+        <v>46116</v>
+      </c>
+      <c r="E79" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G79" s="27" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="11">
+        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
+        <v>-1</v>
+      </c>
+      <c r="C80" t="s">
         <v>67</v>
       </c>
-      <c r="D79" s="12"/>
-      <c r="E79" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G79" s="27"/>
-    </row>
-    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="11" t="str">
-        <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v/>
-      </c>
-      <c r="C80" t="s">
-        <v>68</v>
-      </c>
-      <c r="D80" s="12"/>
+      <c r="D80" s="12">
+        <v>46116</v>
+      </c>
       <c r="E80" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F80" s="11" t="str">
-        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v/>
-      </c>
-      <c r="G80" s="27"/>
+      <c r="F80" s="11">
+        <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
+        <v>-1</v>
+      </c>
+      <c r="G80" s="27" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="str">
@@ -2898,7 +2978,7 @@
         <v/>
       </c>
       <c r="C81" s="22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D81" s="23"/>
       <c r="E81" s="24"/>
@@ -2914,10 +2994,10 @@
         <v>-1</v>
       </c>
       <c r="C82" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D82" s="12">
-        <v>46114</v>
+        <v>46116</v>
       </c>
       <c r="E82" s="13" t="s">
         <v>10</v>
@@ -2927,7 +3007,7 @@
         <v>-1</v>
       </c>
       <c r="G82" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2936,7 +3016,7 @@
         <v>-1</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D83" s="12">
         <v>46116</v>
@@ -2949,7 +3029,7 @@
         <v>-1</v>
       </c>
       <c r="G83" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2958,7 +3038,7 @@
         <v>-1</v>
       </c>
       <c r="C84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D84" s="12">
         <v>46116</v>
@@ -2971,7 +3051,7 @@
         <v>-1</v>
       </c>
       <c r="G84" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2980,7 +3060,7 @@
         <v>-1</v>
       </c>
       <c r="C85" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D85" s="12">
         <v>46116</v>
@@ -2993,7 +3073,7 @@
         <v>-1</v>
       </c>
       <c r="G85" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3002,7 +3082,7 @@
         <v/>
       </c>
       <c r="C86" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D86" s="23"/>
       <c r="E86" s="24"/>
@@ -3018,7 +3098,7 @@
         <v>-1</v>
       </c>
       <c r="C87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D87" s="12">
         <v>46117</v>
@@ -3031,7 +3111,7 @@
         <v>-1</v>
       </c>
       <c r="G87" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3040,7 +3120,7 @@
         <v>-1</v>
       </c>
       <c r="C88" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D88" s="12">
         <v>46119</v>
@@ -3053,7 +3133,7 @@
         <v>-1</v>
       </c>
       <c r="G88" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3062,7 +3142,7 @@
         <v>-1</v>
       </c>
       <c r="C89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D89" s="12">
         <v>46119</v>
@@ -3075,7 +3155,7 @@
         <v>-1</v>
       </c>
       <c r="G89" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3084,7 +3164,7 @@
         <v>-1</v>
       </c>
       <c r="C90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D90" s="12">
         <v>46119</v>
@@ -3097,7 +3177,7 @@
         <v>-1</v>
       </c>
       <c r="G90" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3106,7 +3186,7 @@
         <v>-1</v>
       </c>
       <c r="C91" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D91" s="12">
         <v>46120</v>
@@ -3119,7 +3199,7 @@
         <v>-1</v>
       </c>
       <c r="G91" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3128,7 +3208,7 @@
         <v>-1</v>
       </c>
       <c r="C92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D92" s="12">
         <v>46120</v>
@@ -3141,7 +3221,7 @@
         <v>-1</v>
       </c>
       <c r="G92" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3150,7 +3230,7 @@
         <v/>
       </c>
       <c r="C93" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D93" s="23"/>
       <c r="E93" s="24"/>
@@ -3166,7 +3246,7 @@
         <v>-1</v>
       </c>
       <c r="C94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D94" s="12">
         <v>46123</v>
@@ -3179,7 +3259,7 @@
         <v>-1</v>
       </c>
       <c r="G94" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3188,7 +3268,7 @@
         <v>-1</v>
       </c>
       <c r="C95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D95" s="12">
         <v>46123</v>
@@ -3201,7 +3281,7 @@
         <v>-1</v>
       </c>
       <c r="G95" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3210,7 +3290,7 @@
         <v>-1</v>
       </c>
       <c r="C96" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D96" s="12">
         <v>46123</v>
@@ -3223,7 +3303,7 @@
         <v>-1</v>
       </c>
       <c r="G96" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3232,7 +3312,7 @@
         <v>-1</v>
       </c>
       <c r="C97" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D97" s="12">
         <v>46123</v>
@@ -3245,7 +3325,7 @@
         <v>-1</v>
       </c>
       <c r="G97" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3254,7 +3334,7 @@
         <v/>
       </c>
       <c r="C98" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D98" s="23"/>
       <c r="E98" s="24"/>
@@ -3270,7 +3350,7 @@
         <v>-1</v>
       </c>
       <c r="C99" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D99" s="12">
         <v>46123</v>
@@ -3283,7 +3363,7 @@
         <v>-1</v>
       </c>
       <c r="G99" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3292,7 +3372,7 @@
         <v>-1</v>
       </c>
       <c r="C100" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D100" s="12">
         <v>46125</v>
@@ -3305,7 +3385,7 @@
         <v>-1</v>
       </c>
       <c r="G100" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3314,7 +3394,7 @@
         <v>-1</v>
       </c>
       <c r="C101" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D101" s="12">
         <v>46125</v>
@@ -3327,7 +3407,7 @@
         <v>-1</v>
       </c>
       <c r="G101" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3336,7 +3416,7 @@
         <v>-1</v>
       </c>
       <c r="C102" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D102" s="12">
         <v>46125</v>
@@ -3349,7 +3429,7 @@
         <v>-1</v>
       </c>
       <c r="G102" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3358,7 +3438,7 @@
         <v/>
       </c>
       <c r="C103" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D103" s="23"/>
       <c r="E103" s="24"/>
@@ -3374,7 +3454,7 @@
         <v>-1</v>
       </c>
       <c r="C104" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D104" s="12">
         <v>46128</v>
@@ -3387,7 +3467,7 @@
         <v>-1</v>
       </c>
       <c r="G104" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3396,7 +3476,7 @@
         <v>-1</v>
       </c>
       <c r="C105" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D105" s="12">
         <v>46128</v>
@@ -3409,7 +3489,7 @@
         <v>-1</v>
       </c>
       <c r="G105" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3418,7 +3498,7 @@
         <v>-1</v>
       </c>
       <c r="C106" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D106" s="12">
         <v>46128</v>
@@ -3431,7 +3511,7 @@
         <v>-1</v>
       </c>
       <c r="G106" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3440,7 +3520,7 @@
         <v>-1</v>
       </c>
       <c r="C107" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D107" s="12">
         <v>46128</v>
@@ -3453,7 +3533,7 @@
         <v>-1</v>
       </c>
       <c r="G107" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3462,7 +3542,7 @@
         <v/>
       </c>
       <c r="C108" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D108" s="23"/>
       <c r="E108" s="24"/>
@@ -3478,7 +3558,7 @@
         <v>-1</v>
       </c>
       <c r="C109" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D109" s="12">
         <v>46133</v>
@@ -3491,7 +3571,7 @@
         <v>-1</v>
       </c>
       <c r="G109" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3500,7 +3580,7 @@
         <v>-1</v>
       </c>
       <c r="C110" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D110" s="12">
         <v>46133</v>
@@ -3513,7 +3593,7 @@
         <v>-1</v>
       </c>
       <c r="G110" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3522,7 +3602,7 @@
         <v/>
       </c>
       <c r="C111" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D111" s="23"/>
       <c r="E111" s="24"/>
@@ -3538,7 +3618,7 @@
         <v>-1</v>
       </c>
       <c r="C112" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D112" s="12">
         <v>46135</v>
@@ -3551,7 +3631,7 @@
         <v>-1</v>
       </c>
       <c r="G112" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3560,7 +3640,7 @@
         <v>-1</v>
       </c>
       <c r="C113" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D113" s="12">
         <v>46142</v>
@@ -3573,7 +3653,7 @@
         <v>-1</v>
       </c>
       <c r="G113" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3582,7 +3662,7 @@
         <v>-1</v>
       </c>
       <c r="C114" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D114" s="12">
         <v>46142</v>
@@ -3595,7 +3675,7 @@
         <v>-1</v>
       </c>
       <c r="G114" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3604,7 +3684,7 @@
         <v>-1</v>
       </c>
       <c r="C115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D115" s="12">
         <v>46142</v>
@@ -3617,7 +3697,7 @@
         <v>-1</v>
       </c>
       <c r="G115" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="116" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3626,7 +3706,7 @@
         <v/>
       </c>
       <c r="C116" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D116" s="23"/>
       <c r="E116" s="24"/>
@@ -3642,7 +3722,7 @@
         <v>-1</v>
       </c>
       <c r="C117" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D117" s="12">
         <v>46156</v>
@@ -3655,7 +3735,7 @@
         <v>-1</v>
       </c>
       <c r="G117" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3664,7 +3744,7 @@
         <v>-1</v>
       </c>
       <c r="C118" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D118" s="12">
         <v>46156</v>
@@ -3677,7 +3757,7 @@
         <v>-1</v>
       </c>
       <c r="G118" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3686,7 +3766,7 @@
         <v/>
       </c>
       <c r="C119" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D119" s="23"/>
       <c r="E119" s="24"/>
@@ -3702,7 +3782,7 @@
         <v>-1</v>
       </c>
       <c r="C120" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D120" s="12">
         <v>46163</v>
@@ -3715,7 +3795,7 @@
         <v>-1</v>
       </c>
       <c r="G120" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3724,7 +3804,7 @@
         <v>-1</v>
       </c>
       <c r="C121" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D121" s="12">
         <v>46170</v>
@@ -3737,7 +3817,7 @@
         <v>-1</v>
       </c>
       <c r="G121" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3746,7 +3826,7 @@
         <v>-1</v>
       </c>
       <c r="C122" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D122" s="12">
         <v>46170</v>
@@ -3759,7 +3839,7 @@
         <v>-1</v>
       </c>
       <c r="G122" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3768,7 +3848,7 @@
         <v>-1</v>
       </c>
       <c r="C123" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D123" s="12">
         <v>46170</v>
@@ -3781,7 +3861,7 @@
         <v>-1</v>
       </c>
       <c r="G123" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="124" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3790,7 +3870,7 @@
         <v/>
       </c>
       <c r="C124" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D124" s="23"/>
       <c r="E124" s="24"/>
@@ -3806,7 +3886,7 @@
         <v>-1</v>
       </c>
       <c r="C125" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D125" s="12">
         <v>46177</v>
@@ -3819,7 +3899,7 @@
         <v>-1</v>
       </c>
       <c r="G125" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="126" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3828,7 +3908,7 @@
         <v>-1</v>
       </c>
       <c r="C126" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D126" s="12">
         <v>46177</v>
@@ -3841,7 +3921,7 @@
         <v>-1</v>
       </c>
       <c r="G126" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3850,7 +3930,7 @@
         <v>-1</v>
       </c>
       <c r="C127" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D127" s="12">
         <v>46177</v>
@@ -3863,7 +3943,7 @@
         <v>-1</v>
       </c>
       <c r="G127" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3872,7 +3952,7 @@
         <v>-1</v>
       </c>
       <c r="C128" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D128" s="12">
         <v>46177</v>
@@ -3885,7 +3965,7 @@
         <v>-1</v>
       </c>
       <c r="G128" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3894,7 +3974,7 @@
         <v>-1</v>
       </c>
       <c r="C129" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D129" s="12">
         <v>46177</v>
@@ -3907,7 +3987,7 @@
         <v>-1</v>
       </c>
       <c r="G129" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3916,7 +3996,7 @@
         <v/>
       </c>
       <c r="C130" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D130" s="23"/>
       <c r="E130" s="24"/>
@@ -3932,7 +4012,7 @@
         <v>-1</v>
       </c>
       <c r="C131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D131" s="12">
         <v>46185</v>
@@ -3945,7 +4025,7 @@
         <v>-1</v>
       </c>
       <c r="G131" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3954,7 +4034,7 @@
         <v>-1</v>
       </c>
       <c r="C132" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D132" s="12">
         <v>46185</v>
@@ -3967,7 +4047,7 @@
         <v>-1</v>
       </c>
       <c r="G132" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3976,7 +4056,7 @@
         <v>-1</v>
       </c>
       <c r="C133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D133" s="12">
         <v>46185</v>
@@ -3989,7 +4069,7 @@
         <v>-1</v>
       </c>
       <c r="G133" s="27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change complitions status of pahse 1.2
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A883F74D-4F2F-4145-870A-C83CB6069CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{425D2297-23CE-4B84-B394-83AA99660D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="149">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>Gesamt-XP pro User berechnen/abrufen</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -1334,8 +1337,8 @@
   </sheetPr>
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1551,7 +1554,7 @@
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -1560,11 +1563,11 @@
         <v>46079</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>10</v>
+        <v>134</v>
       </c>
       <c r="F13" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G13" s="27" t="s">
         <v>137</v>
@@ -1573,7 +1576,7 @@
     <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -1582,11 +1585,11 @@
         <v>46079</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="F14" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G14" s="27" t="s">
         <v>137</v>
@@ -1595,7 +1598,7 @@
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -1604,11 +1607,11 @@
         <v>46079</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="F15" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="27" t="s">
         <v>139</v>
@@ -1617,7 +1620,7 @@
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -1626,11 +1629,11 @@
         <v>46079</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="F16" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G16" s="27" t="s">
         <v>139</v>

</xml_diff>

<commit_message>
Add USE-Case Subdivision / Structure
</commit_message>
<xml_diff>
--- a/Documentation/project-plan.xlsx
+++ b/Documentation/project-plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebiru\code\Informatik-2.Jahr\IPT6.1\IPT6.1-Productivity-Game\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sanji\Documents\GitHub\IPT6.1-Productivity-Game\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF06085-3960-44B6-A88F-A38FFD2B302A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8ECC97-10A1-4D8E-822F-998F457C238C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Idea Planner" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
   <definedNames>
     <definedName name="ColumnTitle1">Tasks[[#Headers],[ Task Status Indicator]]</definedName>
     <definedName name="ColumnTitleRegion1..G5.1">'Idea Planner'!$B$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Idea Planner'!$6:$6</definedName>
     <definedName name="PlanDueDate">'Idea Planner'!$E$3</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Idea Planner'!$6:$6</definedName>
     <definedName name="RowTitleRegion1..E3">'Idea Planner'!$D$2</definedName>
     <definedName name="RowTitleRegion2..G3">'Idea Planner'!$F$2</definedName>
   </definedNames>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="149">
   <si>
     <t>Idea Planner</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>Gesamt-XP pro User berechnen/abrufen</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
@@ -837,26 +840,26 @@
     </xf>
   </cellXfs>
   <cellStyles count="20">
-    <cellStyle name="Calculation" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Berechnung" xfId="16" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Center aligned" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Comma" xfId="10" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="11" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="12" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="13" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Dezimal [0]" xfId="11" builtinId="6" customBuiltin="1"/>
     <cellStyle name="Due Date" xfId="18" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Explanatory Text" xfId="7" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="14" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Erklärender Text" xfId="7" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Komma" xfId="10" builtinId="3" customBuiltin="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Plan Due Date" xfId="8" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Prozent" xfId="14" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Status Icon Text" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Task Indicator" xfId="17" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Überschrift 4" xfId="15" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Währung" xfId="12" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Währung [0]" xfId="13" builtinId="7" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1334,27 +1337,27 @@
   </sheetPr>
   <dimension ref="B1:G133"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.54296875" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
     <col min="2" max="2" width="1" customWidth="1"/>
-    <col min="3" max="3" width="42.54296875" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="5" max="5" width="22.54296875" customWidth="1"/>
+    <col min="3" max="3" width="42.5546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.5546875" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="7" width="43.453125" customWidth="1"/>
-    <col min="8" max="8" width="2.54296875" customWidth="1"/>
+    <col min="7" max="7" width="43.44140625" customWidth="1"/>
+    <col min="8" max="8" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="33"/>
       <c r="C1" s="33"/>
     </row>
-    <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:7" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
@@ -1368,7 +1371,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:7" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="34"/>
       <c r="C3" s="34"/>
       <c r="D3" s="10" t="s">
@@ -1384,7 +1387,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:7" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="35" t="s">
         <v>3</v>
       </c>
@@ -1396,7 +1399,7 @@
       <c r="F4" s="35"/>
       <c r="G4" s="35"/>
     </row>
-    <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="36" t="s">
         <v>145</v>
       </c>
@@ -1408,7 +1411,7 @@
       <c r="F5" s="36"/>
       <c r="G5" s="36"/>
     </row>
-    <row r="6" spans="2:7" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1428,7 +1431,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -1444,7 +1447,7 @@
       </c>
       <c r="G7" s="26"/>
     </row>
-    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1466,7 +1469,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1488,7 +1491,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1510,7 +1513,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1532,7 +1535,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -1548,7 +1551,7 @@
       </c>
       <c r="G12" s="28"/>
     </row>
-    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1570,7 +1573,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1592,7 +1595,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1614,7 +1617,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>1</v>
@@ -1636,10 +1639,10 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
         <v>21</v>
@@ -1648,17 +1651,17 @@
         <v>46079</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>10</v>
+        <v>148</v>
       </c>
       <c r="F17" s="11">
         <f ca="1">IFERROR(IF(ISBLANK(Tasks[[#This Row],[Due Date]]),"",IF(Tasks[[#This Row],[Done?]]="Yes",1,IF(OR(Tasks[[#This Row],[Due Date]]&gt;PlanDueDate,Tasks[[#This Row],[Done?]]="No"),-1,IF(OR(OR(Tasks[[#This Row],[Due Date]]=TODAY(),Tasks[[#This Row],[Due Date]]=PlanDueDate),Tasks[[#This Row],[Done?]]="Pending"),0,"")))),"")</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -1674,7 +1677,7 @@
       </c>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1696,7 +1699,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1718,7 +1721,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1740,7 +1743,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1762,7 +1765,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1784,7 +1787,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1806,7 +1809,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1828,7 +1831,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -1844,7 +1847,7 @@
       </c>
       <c r="G26" s="25"/>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1866,7 +1869,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1888,7 +1891,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -1904,7 +1907,7 @@
       </c>
       <c r="G29" s="25"/>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1926,7 +1929,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -1942,7 +1945,7 @@
       </c>
       <c r="G31" s="17"/>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1964,7 +1967,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -1986,7 +1989,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2008,7 +2011,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2030,7 +2033,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2046,7 +2049,7 @@
       </c>
       <c r="G36" s="26"/>
     </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2068,7 +2071,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2090,7 +2093,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2112,7 +2115,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2128,7 +2131,7 @@
       </c>
       <c r="G40" s="26"/>
     </row>
-    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2150,7 +2153,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2172,7 +2175,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2194,7 +2197,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2216,7 +2219,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2238,7 +2241,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2254,7 +2257,7 @@
       </c>
       <c r="G46" s="29"/>
     </row>
-    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2276,7 +2279,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B48" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2298,7 +2301,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B49" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2320,7 +2323,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2342,7 +2345,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2364,7 +2367,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2386,7 +2389,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2408,7 +2411,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2430,7 +2433,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B55" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2452,7 +2455,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B56" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2468,7 +2471,7 @@
       </c>
       <c r="G56" s="29"/>
     </row>
-    <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B57" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2490,7 +2493,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2512,7 +2515,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B59" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2534,7 +2537,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B60" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2556,7 +2559,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B61" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2572,7 +2575,7 @@
       </c>
       <c r="G61" s="29"/>
     </row>
-    <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B62" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2594,7 +2597,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B63" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2616,7 +2619,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B64" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2638,7 +2641,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B65" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2654,7 +2657,7 @@
       </c>
       <c r="G65" s="29"/>
     </row>
-    <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B66" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2676,7 +2679,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B67" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2698,7 +2701,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B68" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2720,7 +2723,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B69" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2742,7 +2745,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B70" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2758,7 +2761,7 @@
       </c>
       <c r="G70" s="29"/>
     </row>
-    <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2780,7 +2783,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B72" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2802,7 +2805,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B73" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2824,7 +2827,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2846,7 +2849,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2868,7 +2871,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2884,7 +2887,7 @@
       </c>
       <c r="G76" s="29"/>
     </row>
-    <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B77" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2906,7 +2909,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B78" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2928,7 +2931,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B79" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2950,7 +2953,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B80" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -2972,7 +2975,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -2988,7 +2991,7 @@
       </c>
       <c r="G81" s="29"/>
     </row>
-    <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3010,7 +3013,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B83" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3032,7 +3035,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B84" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3054,7 +3057,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B85" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3076,7 +3079,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B86" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3092,7 +3095,7 @@
       </c>
       <c r="G86" s="29"/>
     </row>
-    <row r="87" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B87" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3114,7 +3117,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B88" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3136,7 +3139,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B89" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3158,7 +3161,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B90" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3180,7 +3183,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B91" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3202,7 +3205,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3224,7 +3227,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B93" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="G93" s="29"/>
     </row>
-    <row r="94" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B94" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3262,7 +3265,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3284,7 +3287,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B96" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3306,7 +3309,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3328,7 +3331,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3344,7 +3347,7 @@
       </c>
       <c r="G98" s="29"/>
     </row>
-    <row r="99" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3366,7 +3369,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3388,7 +3391,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B101" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3410,7 +3413,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B102" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3432,7 +3435,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B103" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3448,7 +3451,7 @@
       </c>
       <c r="G103" s="29"/>
     </row>
-    <row r="104" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B104" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3470,7 +3473,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B105" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3492,7 +3495,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B106" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3514,7 +3517,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B107" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3536,7 +3539,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B108" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3552,7 +3555,7 @@
       </c>
       <c r="G108" s="29"/>
     </row>
-    <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B109" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3574,7 +3577,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3596,7 +3599,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B111" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3612,7 +3615,7 @@
       </c>
       <c r="G111" s="29"/>
     </row>
-    <row r="112" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3634,7 +3637,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B113" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3656,7 +3659,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3678,7 +3681,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B115" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3700,7 +3703,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="116" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B116" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3716,7 +3719,7 @@
       </c>
       <c r="G116" s="29"/>
     </row>
-    <row r="117" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B117" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3738,7 +3741,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B118" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3760,7 +3763,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B119" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3776,7 +3779,7 @@
       </c>
       <c r="G119" s="29"/>
     </row>
-    <row r="120" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B120" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3798,7 +3801,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B121" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3820,7 +3823,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B122" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3842,7 +3845,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B123" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3864,7 +3867,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="124" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B124" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -3880,7 +3883,7 @@
       </c>
       <c r="G124" s="29"/>
     </row>
-    <row r="125" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B125" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3902,7 +3905,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="126" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B126" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3924,7 +3927,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="127" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B127" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3946,7 +3949,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="128" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B128" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3968,7 +3971,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="129" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B129" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -3990,7 +3993,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="130" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B130" s="11" t="str">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v/>
@@ -4006,7 +4009,7 @@
       </c>
       <c r="G130" s="29"/>
     </row>
-    <row r="131" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B131" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -4028,7 +4031,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B132" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>
@@ -4050,7 +4053,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B133" s="11">
         <f ca="1">Tasks[[#This Row],[Status Icon]]</f>
         <v>-1</v>

</xml_diff>